<commit_message>
Gestion projet | modif | MAJ suivie des évolutions
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://arcelormittal-my.sharepoint.com/personal/u049298_arcelormittal_es1/Documents/1_Administratif/Perso/projetWebRPG/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard\Desktop\CESI\PYTHON\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="358" documentId="8_{535D38EE-B244-4780-AED4-3C048858F5B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{28B41C0F-E72A-4B4A-9BAB-E1438CC077AE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" xr2:uid="{A052D7F7-200B-4224-AA67-DF3328173750}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Evolutions" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="Info Lvl" sheetId="2" r:id="rId3"/>
     <sheet name="Feuil2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -294,12 +293,15 @@
   </si>
   <si>
     <t>compétence physique(exemple charge)</t>
+  </si>
+  <si>
+    <t>En prod</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
@@ -335,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -363,26 +365,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -422,7 +439,6 @@
         <sz val="8"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -434,6 +450,22 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -443,7 +475,76 @@
         <sz val="8"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -458,7 +559,6 @@
         <sz val="8"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -473,113 +573,9 @@
         <sz val="8"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -598,49 +594,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41EA5FFA-96C2-45C4-87CA-8EF6AB511A6E}" name="Tableau1" displayName="Tableau1" ref="B2:H30" totalsRowShown="0" headerRowDxfId="23" dataDxfId="7">
-  <autoFilter ref="B2:H30" xr:uid="{ADA84220-FEF1-46FA-9353-9845D6B908FE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:H30" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B2:H30"/>
   <sortState ref="B3:H30">
     <sortCondition ref="D2:D30"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6F977295-2A95-40BB-9B94-B45C44CCCDEB}" name="Fonctionnalité" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C3F52030-6F97-4647-9D36-56316EB9BD9C}" name="Desciption" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{49FDEFAF-8B03-4311-B6DF-A372DE808374}" name="Priorité" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{A9B9A0AF-8B1D-484C-BCB4-57DAA69E8A95}" name="Etat" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{FFAA8598-EDC4-4157-915A-B5B13604D9F9}" name="Date début" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{B01C389B-049F-4EB0-A94C-332BCF0446E4}" name="Date fin" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{6B7733ED-E352-443B-92AE-AF3CF27AB38F}" name="Dev" dataDxfId="8"/>
+    <tableColumn id="1" name="Fonctionnalité" dataDxfId="21"/>
+    <tableColumn id="2" name="Desciption" dataDxfId="20"/>
+    <tableColumn id="5" name="Priorité" dataDxfId="19"/>
+    <tableColumn id="3" name="Etat" dataDxfId="18"/>
+    <tableColumn id="6" name="Date début" dataDxfId="17"/>
+    <tableColumn id="7" name="Date fin" dataDxfId="16"/>
+    <tableColumn id="9" name="Dev" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9A44EE58-74AC-429A-8FBF-7A4CE010128F}" name="Tableau4" displayName="Tableau4" ref="B2:F6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="B2:F6" xr:uid="{401C3DD0-F4A8-423D-B51E-509C04CC771D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B2:F6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="B2:F6"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{6C24FCBB-593C-4671-A2C4-C927412F9E83}" name="Bug" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{62CCA482-5A5A-4C29-9B42-3E63D51F682C}" name="Cause"/>
-    <tableColumn id="3" xr3:uid="{536B966E-FEDE-4471-8306-2F1E1D542526}" name="Etat" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{AAEC5031-52E7-4586-BC76-97FB6A70BDC1}" name="Date report" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6CDB48B8-325E-48F5-AD68-C75D2C896F41}" name="Date closure" dataDxfId="2"/>
+    <tableColumn id="1" name="Bug" dataDxfId="12"/>
+    <tableColumn id="2" name="Cause"/>
+    <tableColumn id="3" name="Etat" dataDxfId="11"/>
+    <tableColumn id="4" name="Date report" dataDxfId="10"/>
+    <tableColumn id="5" name="Date closure" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB772001-B0A9-40D9-9B9C-72ED5D0AFE0C}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="B2:D32" xr:uid="{F853BE75-B3ED-4974-BFBA-4568633A9E79}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="B2:D32"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D01CFAEC-04FF-40BF-A086-0A8645C9259C}" name="LVL" dataDxfId="21">
+    <tableColumn id="1" name="LVL" dataDxfId="7">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{8BBA4156-57BD-4F3C-A78C-C648A621F52D}" name="Xp avant le niveau suivant" dataDxfId="20">
+    <tableColumn id="2" name="Xp avant le niveau suivant" dataDxfId="6">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{42F1C891-9983-429A-A3C3-6FF1B9B6A278}" name="XP depuis le début du jeu" dataDxfId="19">
+    <tableColumn id="3" name="XP depuis le début du jeu" dataDxfId="5">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -649,12 +645,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C3B9FDDD-0B79-44FC-A2CA-BC4DE9DA8644}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="H2:J3" xr:uid="{D8BF23CC-243B-4C23-AC1B-183899852105}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="H2:J3"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A7161BCA-A8C1-48DC-B6F2-0BA2A1EF7E1E}" name="lvl actuelle" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{BBFD8630-2B34-45EA-9885-76BE11B222E7}" name="xp actuelle" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{9162B359-A327-45E2-9CC1-ABE51195BEC1}" name="up ou pas ?" dataDxfId="14">
+    <tableColumn id="1" name="lvl actuelle" dataDxfId="2"/>
+    <tableColumn id="2" name="xp actuelle" dataDxfId="1"/>
+    <tableColumn id="3" name="up ou pas ?" dataDxfId="0">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -958,11 +954,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5644FFC1-9C62-4CC1-8A1D-5DD5328F5C12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1031,10 +1027,14 @@
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="F4" s="11">
+        <v>43863</v>
+      </c>
+      <c r="G4" s="11">
+        <v>43863</v>
+      </c>
       <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1066,7 +1066,9 @@
       <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="7"/>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7" t="s">
@@ -1103,7 +1105,9 @@
       <c r="D8" s="7">
         <v>1</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -1482,7 +1486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DD9C30-3811-4B83-8E3D-54C33354DE57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1550,7 +1554,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE394F6-28BC-4CAA-B44B-BC3D6CFFFD2C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J1401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6137,7 +6141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF11D46-F7A4-4E88-A41D-D53FFE064777}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6210,9 +6214,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6419,27 +6426,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6464,9 +6459,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Loot display | Add | Stuff location on modal and inventory & rarity of stuff in inventory
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richard\Desktop\CESI\PYTHON\projetWebRPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8C6DE0-00C1-493F-A428-CFA3AF2F6940}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evolutions" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Info Lvl" sheetId="2" r:id="rId3"/>
     <sheet name="Feuil2" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -226,9 +227,6 @@
     <t>Descendre le taux de drop des legendaires a 1/100</t>
   </si>
   <si>
-    <t>Les rareté des equipement dans l'équipement</t>
-  </si>
-  <si>
     <t>quand on boit une potion ne pas dépaser son PV MAX</t>
   </si>
   <si>
@@ -253,9 +251,6 @@
     <t>Date closure</t>
   </si>
   <si>
-    <t>Ecrire les les noms des slots dans le modal</t>
-  </si>
-  <si>
     <t>Cause</t>
   </si>
   <si>
@@ -296,12 +291,21 @@
   </si>
   <si>
     <t>En prod</t>
+  </si>
+  <si>
+    <t>Ecrire les les noms des slots dans l'inventaire</t>
+  </si>
+  <si>
+    <t>DevMerge</t>
+  </si>
+  <si>
+    <t>NassimDev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
@@ -594,49 +598,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:H30" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B2:H30"/>
-  <sortState ref="B3:H30">
-    <sortCondition ref="D2:D30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B2:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="B3:H29">
+    <sortCondition ref="D2:D29"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" name="Fonctionnalité" dataDxfId="21"/>
-    <tableColumn id="2" name="Desciption" dataDxfId="20"/>
-    <tableColumn id="5" name="Priorité" dataDxfId="19"/>
-    <tableColumn id="3" name="Etat" dataDxfId="18"/>
-    <tableColumn id="6" name="Date début" dataDxfId="17"/>
-    <tableColumn id="7" name="Date fin" dataDxfId="16"/>
-    <tableColumn id="9" name="Dev" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="B2:F6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="B2:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:F6" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+  <autoFilter ref="B2:F6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Bug" dataDxfId="12"/>
-    <tableColumn id="2" name="Cause"/>
-    <tableColumn id="3" name="Etat" dataDxfId="11"/>
-    <tableColumn id="4" name="Date report" dataDxfId="10"/>
-    <tableColumn id="5" name="Date closure" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="B2:D32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="B2:D32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="LVL" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="7">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Xp avant le niveau suivant" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="6">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="XP depuis le début du jeu" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="5">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -645,12 +649,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="H2:J3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="H2:J3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="lvl actuelle" dataDxfId="2"/>
-    <tableColumn id="2" name="xp actuelle" dataDxfId="1"/>
-    <tableColumn id="3" name="up ou pas ?" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="0">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -954,11 +958,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F4" s="11">
         <v>43863</v>
@@ -1067,10 +1071,14 @@
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="F6" s="11">
+        <v>43863</v>
+      </c>
+      <c r="G6" s="11">
+        <v>43863</v>
+      </c>
       <c r="H6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1100,17 +1108,23 @@
         <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="F8" s="11">
+        <v>43864</v>
+      </c>
+      <c r="G8" s="11">
+        <v>43864</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B9" s="6" t="s">
@@ -1125,8 +1139,8 @@
       <c r="E9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1140,26 +1154,38 @@
         <v>2</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="F10" s="11">
+        <v>43864</v>
+      </c>
+      <c r="G10" s="11">
+        <v>43864</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="7">
         <v>2</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+        <v>87</v>
+      </c>
+      <c r="F11" s="11">
+        <v>43864</v>
+      </c>
+      <c r="G11" s="11">
+        <v>43864</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B12" s="6" t="s">
@@ -1182,7 +1208,7 @@
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>55</v>
@@ -1202,7 +1228,7 @@
         <v>58</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="7">
         <v>2</v>
@@ -1282,25 +1308,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B19" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="D19" s="7">
-        <v>3</v>
-      </c>
-      <c r="E19" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B20" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D20" s="7">
         <v>4</v>
@@ -1310,33 +1340,33 @@
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="H20" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B21" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D21" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B22" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" s="7">
         <v>5</v>
@@ -1348,18 +1378,18 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D23" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1367,27 +1397,27 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D24" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B25" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" s="7">
         <v>7</v>
@@ -1399,15 +1429,15 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D26" s="7">
-        <v>7</v>
+        <v>1000</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>9</v>
@@ -1418,10 +1448,10 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D27" s="7">
         <v>1000</v>
@@ -1435,14 +1465,10 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="7">
-        <v>1000</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
         <v>9</v>
       </c>
@@ -1450,9 +1476,9 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B29" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
@@ -1462,19 +1488,6 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1486,11 +1499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1506,19 +1519,19 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
@@ -1529,10 +1542,10 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="33.75" x14ac:dyDescent="0.2">
@@ -1554,7 +1567,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:J1401"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6141,7 +6154,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6156,55 +6169,55 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
         <v>78</v>
       </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
       <c r="E3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
         <v>77</v>
       </c>
-      <c r="C5" t="s">
-        <v>79</v>
-      </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -6214,12 +6227,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6426,15 +6436,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6459,18 +6481,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Project Management | Update | Bug Closed
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y0652097\Desktop\CESIproject\PythonProject\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ECB0270-F648-4321-B1C6-BD28AF5F9768}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1728BDDE-7A7C-442C-9FEB-355320DC4986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evolutions" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -302,14 +302,32 @@
     <t>NassimDev</t>
   </si>
   <si>
-    <t>En cours</t>
+    <t>Génération des enemies fait par rapport au carac brut du personnage</t>
+  </si>
+  <si>
+    <t>Cosed</t>
+  </si>
+  <si>
+    <t>modal item qui ne se vide pas surement a cause du spam</t>
+  </si>
+  <si>
+    <t>ecrire les les noms des slots</t>
+  </si>
+  <si>
+    <t>les rareté des equipement mis</t>
+  </si>
+  <si>
+    <t>ecrire dans la modal dans quel slot ira l'item</t>
+  </si>
+  <si>
+    <t>attendre la réponse json avant de remettre le bouton play round (faire comme next stage le suprimmer et a la fin le remettre)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -328,6 +346,17 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -351,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -385,11 +414,44 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -398,11 +460,86 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
         <color auto="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -414,10 +551,32 @@
         <vertAlign val="baseline"/>
         <sz val="8"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -532,15 +691,12 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="8"/>
+        <color auto="1"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -551,132 +707,10 @@
         <vertAlign val="baseline"/>
         <sz val="8"/>
         <name val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -692,49 +726,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="B2:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="B3:H29">
     <sortCondition ref="D2:D29"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:F7" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="B2:F7" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:F16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="B2:F16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B2:D32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="7">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="22">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="6">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="5">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -743,12 +777,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="H2:J3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="0">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -757,7 +791,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1055,11 +1089,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="10"/>
     <col min="2" max="2" width="47.83203125" style="10" bestFit="1" customWidth="1"/>
@@ -1072,7 +1106,7 @@
     <col min="9" max="16384" width="2.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1129,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:13" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1114,7 +1148,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:13" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" ht="78.75" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1137,7 +1171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:13" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1156,7 +1190,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>63</v>
       </c>
@@ -1177,7 +1211,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:13" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1197,7 +1231,7 @@
       </c>
       <c r="M7" s="12"/>
     </row>
-    <row r="8" spans="2:13" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>53</v>
       </c>
@@ -1220,7 +1254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1239,7 +1273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>59</v>
       </c>
@@ -1260,7 +1294,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>86</v>
       </c>
@@ -1281,7 +1315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:13" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1300,7 +1334,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>67</v>
       </c>
@@ -1317,7 +1351,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>58</v>
       </c>
@@ -1334,7 +1368,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="2:13" s="10" customFormat="1" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>18</v>
       </c>
@@ -1351,7 +1385,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="2:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>57</v>
       </c>
@@ -1372,7 +1406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
@@ -1391,7 +1425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:8" ht="45" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>24</v>
       </c>
@@ -1410,7 +1444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:8" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1427,7 +1461,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="2:8" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>26</v>
       </c>
@@ -1446,7 +1480,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:8" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
@@ -1463,7 +1497,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="2:8" s="10" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:8" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>30</v>
       </c>
@@ -1480,7 +1514,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1497,7 +1531,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>37</v>
       </c>
@@ -1514,7 +1548,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="2:8" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>39</v>
       </c>
@@ -1531,7 +1565,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>43</v>
       </c>
@@ -1548,7 +1582,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>41</v>
       </c>
@@ -1565,7 +1599,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="2:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>56</v>
       </c>
@@ -1578,7 +1612,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="2:8" s="10" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:8" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
         <v>60</v>
       </c>
@@ -1602,16 +1636,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="8"/>
-    <col min="2" max="2" width="31.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="8" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" style="8" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="8" customWidth="1"/>
@@ -1619,7 +1653,7 @@
     <col min="7" max="16384" width="2.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
         <v>69</v>
       </c>
@@ -1636,36 +1670,169 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="13">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" s="8" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="E4" s="13">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="E5" s="13">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="13">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F7" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
         <v>89</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F8" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E9" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F9" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E10" s="13">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F11" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F12" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F13" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F14" s="13">
+        <v>43865</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="B15" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="13">
+        <v>43860</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="B16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="13">
+        <v>43860</v>
+      </c>
+      <c r="F16" s="13">
+        <v>43865</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +1852,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1"/>
     <col min="2" max="2" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -6272,7 +6439,7 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
@@ -6338,12 +6505,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6550,15 +6714,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6583,18 +6759,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Debug | Stuff display | Change | Consumables panel order: Name - quantity - button, corrected in main.js on adding consumables
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y0652097\Desktop\CESIproject\PythonProject\projetWebRPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1728BDDE-7A7C-442C-9FEB-355320DC4986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621DEDF4-1805-4FB0-A7C0-0550789DD78D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -791,7 +791,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1093,7 +1093,7 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="10"/>
     <col min="2" max="2" width="47.83203125" style="10" bestFit="1" customWidth="1"/>
@@ -1315,7 +1315,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1636,13 +1636,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:F16"/>
+  <dimension ref="B2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="8"/>
     <col min="2" max="2" width="35.33203125" style="8" customWidth="1"/>
@@ -1698,7 +1698,7 @@
         <v>43860</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
@@ -1833,6 +1833,11 @@
       </c>
       <c r="F16" s="13">
         <v>43865</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1852,7 +1857,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1"/>
     <col min="2" max="2" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -6439,7 +6444,7 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
@@ -6505,9 +6510,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6714,27 +6722,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6759,9 +6755,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Project Management | Update | Debug
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y0652097\Desktop\CESIproject\PythonProject\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621DEDF4-1805-4FB0-A7C0-0550789DD78D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3D72F0-9722-446D-A4D3-E1A2C3BDF91A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Génération des enemies fait par rapport au carac brut du personnage</t>
   </si>
   <si>
-    <t>Cosed</t>
-  </si>
-  <si>
     <t>modal item qui ne se vide pas surement a cause du spam</t>
   </si>
   <si>
@@ -321,6 +318,21 @@
   </si>
   <si>
     <t>attendre la réponse json avant de remettre le bouton play round (faire comme next stage le suprimmer et a la fin le remettre)</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Abort</t>
+  </si>
+  <si>
+    <t>Commentary</t>
+  </si>
+  <si>
+    <t>Pas la peine finalement car on a régler autrement le probleme en resolvant les spam play round item et nextstage</t>
+  </si>
+  <si>
+    <t>On ne sait pas comment ai dû ce probleme mais il a du être resolu en même temps que le spam playRound dropItem</t>
   </si>
 </sst>
 </file>
@@ -380,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -419,11 +431,57 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -451,24 +509,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -726,49 +766,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="B2:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="B3:H29">
     <sortCondition ref="D2:D29"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:F16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B2:F16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:G16" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="B2:G16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="B2:D32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="9">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="8">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="7">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -777,12 +818,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="H2:J3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="2">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -791,7 +832,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1093,7 +1134,7 @@
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="10"/>
     <col min="2" max="2" width="47.83203125" style="10" bestFit="1" customWidth="1"/>
@@ -1315,7 +1356,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1636,13 +1677,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:F22"/>
+  <dimension ref="B2:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="8"/>
     <col min="2" max="2" width="35.33203125" style="8" customWidth="1"/>
@@ -1650,10 +1691,11 @@
     <col min="4" max="4" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="8" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="2.6640625" style="8"/>
+    <col min="7" max="7" width="45" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="2.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="8" t="s">
         <v>69</v>
       </c>
@@ -1669,8 +1711,11 @@
       <c r="F2" s="8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>54</v>
       </c>
@@ -1678,40 +1723,64 @@
       <c r="E3" s="13">
         <v>43860</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="6" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>66</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="E4" s="13">
         <v>43860</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="F4" s="13">
+        <v>43865</v>
+      </c>
+      <c r="G4" s="17"/>
+    </row>
+    <row r="5" spans="2:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>61</v>
       </c>
+      <c r="D5" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="E5" s="13">
         <v>43860</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="F5" s="13">
+        <v>43865</v>
+      </c>
+      <c r="G5" s="17"/>
+    </row>
+    <row r="6" spans="2:7" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B6" s="6" t="s">
         <v>62</v>
       </c>
+      <c r="D6" s="8" t="s">
+        <v>95</v>
+      </c>
       <c r="E6" s="13">
         <v>43860</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F6" s="13">
+        <v>43865</v>
+      </c>
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E7" s="13">
         <v>43860</v>
@@ -1719,14 +1788,15 @@
       <c r="F7" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
         <v>89</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E8" s="13">
         <v>43860</v>
@@ -1734,13 +1804,14 @@
       <c r="F8" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>57</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E9" s="13">
         <v>43860</v>
@@ -1748,21 +1819,23 @@
       <c r="F9" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="13">
         <v>43860</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>58</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E11" s="13">
         <v>43860</v>
@@ -1770,13 +1843,14 @@
       <c r="F11" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E12" s="13">
         <v>43860</v>
@@ -1784,13 +1858,14 @@
       <c r="F12" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="17"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E13" s="13">
         <v>43860</v>
@@ -1798,13 +1873,14 @@
       <c r="F13" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E14" s="13">
         <v>43860</v>
@@ -1812,21 +1888,31 @@
       <c r="F14" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="45" x14ac:dyDescent="0.2">
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="E15" s="13">
         <v>43860</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="F15" s="13">
+        <v>43866</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E16" s="13">
         <v>43860</v>
@@ -1834,11 +1920,7 @@
       <c r="F16" s="13">
         <v>43865</v>
       </c>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
+      <c r="G16" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1857,7 +1939,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1"/>
     <col min="2" max="2" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -6444,7 +6526,7 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
@@ -6510,12 +6592,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6722,15 +6801,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6755,18 +6846,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Loot system | Add | generateItem function create random item with 1/3 frequency in dopItem() or when the db is empty
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y0652097\Desktop\CESIproject\PythonProject\projetWebRPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3D72F0-9722-446D-A4D3-E1A2C3BDF91A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7B1945-44B3-4786-800C-E3614E94836C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evolutions" sheetId="1" r:id="rId1"/>
@@ -446,6 +446,34 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -481,34 +509,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -792,24 +792,24 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B2:D32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="7">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="6">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="5">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -818,12 +818,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="H2:J3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="0">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -832,7 +832,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1130,11 +1130,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="10"/>
     <col min="2" max="2" width="47.83203125" style="10" bestFit="1" customWidth="1"/>
@@ -1223,10 +1223,14 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="F5" s="7">
+        <v>43867</v>
+      </c>
+      <c r="G5" s="7">
+        <v>43867</v>
+      </c>
       <c r="H5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1356,7 +1360,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="67.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" ht="56.25" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
@@ -1679,11 +1683,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="8"/>
     <col min="2" max="2" width="35.33203125" style="8" customWidth="1"/>
@@ -1939,7 +1943,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="1"/>
     <col min="2" max="2" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -6526,7 +6530,7 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
@@ -6592,9 +6596,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6801,27 +6808,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6846,9 +6841,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Item Generation | Change | calculPoints function to know how much point based on rarity and level of equipment the nb point to affect if and dispatchPoints to know how to affect points base on the stuff type and the CharacterClass
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7B1945-44B3-4786-800C-E3614E94836C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F90567-E560-4FF3-A3DB-537106B6B059}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evolutions" sheetId="1" r:id="rId1"/>
     <sheet name="Bug reported" sheetId="3" r:id="rId2"/>
     <sheet name="Info Lvl" sheetId="2" r:id="rId3"/>
-    <sheet name="Feuil2" sheetId="4" r:id="rId4"/>
+    <sheet name="Modifcateur info" sheetId="5" r:id="rId4"/>
+    <sheet name="Stuff info" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="138">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -254,42 +255,6 @@
     <t>Cause</t>
   </si>
   <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
-    <t>Magique</t>
-  </si>
-  <si>
-    <t>Phyisique</t>
-  </si>
-  <si>
-    <t>degat darme</t>
-  </si>
-  <si>
-    <t>physique</t>
-  </si>
-  <si>
-    <t>Compétence</t>
-  </si>
-  <si>
-    <t>Physique/magique</t>
-  </si>
-  <si>
-    <t>Physique</t>
-  </si>
-  <si>
-    <t>type de compétence</t>
-  </si>
-  <si>
-    <t>soin/sort/compétence physique(exemple charge)</t>
-  </si>
-  <si>
-    <t>soin/sort</t>
-  </si>
-  <si>
-    <t>compétence physique(exemple charge)</t>
-  </si>
-  <si>
     <t>En prod</t>
   </si>
   <si>
@@ -333,13 +298,163 @@
   </si>
   <si>
     <t>On ne sait pas comment ai dû ce probleme mais il a du être resolu en même temps que le spam playRound dropItem</t>
+  </si>
+  <si>
+    <t>Valeur carac</t>
+  </si>
+  <si>
+    <t>Rareté</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Legandary</t>
+  </si>
+  <si>
+    <t>Stuff</t>
+  </si>
+  <si>
+    <t>Modificateur overall</t>
+  </si>
+  <si>
+    <t>Modificateur overall base</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Multiplicateur</t>
+  </si>
+  <si>
+    <t>Legendary</t>
+  </si>
+  <si>
+    <t>Modificateur total overall</t>
+  </si>
+  <si>
+    <t>Consomable</t>
+  </si>
+  <si>
+    <t>Nom d'arme</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Stick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bludgeon </t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Bardiche</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Arming sword</t>
+  </si>
+  <si>
+    <t>Katana</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
+  <si>
+    <t>Longsword</t>
+  </si>
+  <si>
+    <t>Saber</t>
+  </si>
+  <si>
+    <t>Rapier</t>
+  </si>
+  <si>
+    <t>Shortsword</t>
+  </si>
+  <si>
+    <t>Battle axe</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>Crossbow</t>
+  </si>
+  <si>
+    <t>Flail</t>
+  </si>
+  <si>
+    <t>Morning star</t>
+  </si>
+  <si>
+    <t>Pernach</t>
+  </si>
+  <si>
+    <t>War hammer</t>
+  </si>
+  <si>
+    <t>Halberd</t>
+  </si>
+  <si>
+    <t>Spear</t>
+  </si>
+  <si>
+    <t>Ranseur</t>
+  </si>
+  <si>
+    <t>Longbow</t>
+  </si>
+  <si>
+    <t>Recurve bow</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Frost</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>intelligence</t>
+  </si>
+  <si>
+    <t>hp</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>agility</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -371,13 +486,33 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -392,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -440,11 +575,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -766,50 +930,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau1" displayName="Tableau1" ref="B2:H29" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="B2:H29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="B3:H29">
     <sortCondition ref="D2:D29"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Fonctionnalité" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Desciption" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Priorité" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Etat" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Date début" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Date fin" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Dev" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:G16" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau4" displayName="Tableau4" ref="B2:G16" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="B2:G16" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Bug" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="B2:D32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="12">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="11">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="5">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="10">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -818,13 +982,60 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="H2:J3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="5">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{75AF6093-40B9-4045-A836-7BE4980C4B82}" name="Tableau5" displayName="Tableau5" ref="B3:C7" totalsRowShown="0">
+  <autoFilter ref="B3:C7" xr:uid="{1BE29893-1322-4690-AA5F-63DF676006D3}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{62EF2871-AA7D-4282-8062-C89624DC7695}" name="Rareté"/>
+    <tableColumn id="2" xr3:uid="{C8BBA3B7-444F-43B1-AFA4-46B868FC8A8E}" name="Modificateur overall"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2097D268-C9D7-444D-AE39-0D44AD7C2BD5}" name="Tableau6" displayName="Tableau6" ref="B10:C14" totalsRowShown="0">
+  <autoFilter ref="B10:C14" xr:uid="{276BC1F8-D857-467C-ACA7-1D093324CFA6}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{DFE081BD-5921-47E0-B435-E29AF1E656ED}" name="Rareté"/>
+    <tableColumn id="2" xr3:uid="{153A6B44-8ED0-4BA7-8A43-77462ECE10CC}" name="Modificateur overall base"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9CF327DF-5BC9-457F-AACB-51597DACBE89}" name="Tableau7" displayName="Tableau7" ref="B17:G37" totalsRowShown="0">
+  <autoFilter ref="B17:G37" xr:uid="{C892CB3D-BF9B-46E5-9300-BEA3BBCAEF09}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{A891AB08-64A9-4A19-B103-7079E9CB00C2}" name="Level"/>
+    <tableColumn id="5" xr3:uid="{8E2D95A1-93C7-4BF2-9825-41B55E7894BB}" name="Multiplicateur" dataDxfId="0">
+      <calculatedColumnFormula>1+(Tableau7[[#This Row],[Level]]-1)*0.25</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BD052409-7DF4-4016-8B8D-C52FEE20CEC8}" name="Common" dataDxfId="4">
+      <calculatedColumnFormula>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{A15D3612-F474-4B9C-8C65-2BB0FE5F4915}" name="Rare" dataDxfId="3">
+      <calculatedColumnFormula>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{3C43E1AB-E1B8-4592-B084-1B3D381FC6B2}" name="Epic" dataDxfId="2">
+      <calculatedColumnFormula>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{B515297F-08B2-4D2C-B3D3-43FD65399196}" name="Legendary" dataDxfId="1">
+      <calculatedColumnFormula>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1130,7 +1341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -1200,7 +1411,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F4" s="7">
         <v>43863</v>
@@ -1223,7 +1434,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F5" s="7">
         <v>43867</v>
@@ -1244,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F6" s="7">
         <v>43863</v>
@@ -1287,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F8" s="7">
         <v>43864</v>
@@ -1327,7 +1538,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F10" s="7">
         <v>43864</v>
@@ -1341,14 +1552,14 @@
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="4">
         <v>2</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F11" s="7">
         <v>43864</v>
@@ -1439,7 +1650,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F16" s="7">
         <v>43864</v>
@@ -1716,7 +1927,7 @@
         <v>71</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="33.75" x14ac:dyDescent="0.2">
@@ -1728,7 +1939,7 @@
         <v>43860</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
@@ -1739,7 +1950,7 @@
         <v>66</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E4" s="13">
         <v>43860</v>
@@ -1754,7 +1965,7 @@
         <v>61</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E5" s="13">
         <v>43860</v>
@@ -1769,7 +1980,7 @@
         <v>62</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E6" s="13">
         <v>43860</v>
@@ -1784,7 +1995,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E7" s="13">
         <v>43860</v>
@@ -1796,11 +2007,11 @@
     </row>
     <row r="8" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B8" s="14" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C8" s="15"/>
       <c r="D8" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E8" s="13">
         <v>43860</v>
@@ -1815,7 +2026,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E9" s="13">
         <v>43860</v>
@@ -1827,7 +2038,7 @@
     </row>
     <row r="10" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E10" s="13">
         <v>43860</v>
@@ -1839,7 +2050,7 @@
         <v>58</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E11" s="13">
         <v>43860</v>
@@ -1851,10 +2062,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E12" s="13">
         <v>43860</v>
@@ -1866,10 +2077,10 @@
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E13" s="13">
         <v>43860</v>
@@ -1881,10 +2092,10 @@
     </row>
     <row r="14" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E14" s="13">
         <v>43860</v>
@@ -1896,10 +2107,10 @@
     </row>
     <row r="15" spans="2:7" ht="45" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E15" s="13">
         <v>43860</v>
@@ -1908,7 +2119,7 @@
         <v>43866</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="22.5" x14ac:dyDescent="0.2">
@@ -1916,7 +2127,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E16" s="13">
         <v>43860</v>
@@ -6523,85 +6734,1709 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E37B00C-9A5C-40C7-9046-353D70841F22}">
+  <dimension ref="B2:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>ROUNDDOWN(B3/4,0)+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">ROUNDDOWN(B4/4,0)+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>36</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>41</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>43</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>46</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>48</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>51</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>52</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>53</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>55</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>56</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>57</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>58</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>59</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>61</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>62</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>63</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>64</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>65</v>
+      </c>
+      <c r="C68">
+        <f t="shared" ref="C68:C131" si="1">ROUNDDOWN(B68/4,0)+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>66</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>67</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>69</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>70</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>71</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>72</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>73</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>74</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>75</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>76</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>77</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>78</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>79</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>80</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>81</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>82</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>83</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>84</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>85</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>86</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>87</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>88</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>89</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>90</v>
+      </c>
+      <c r="C93">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>91</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>92</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>93</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>94</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>95</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>96</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>97</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>98</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>99</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>100</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B2:V37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E5" t="s">
-        <v>84</v>
+        <v>91</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="21"/>
+      <c r="I7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="E8" s="21"/>
+      <c r="I8" t="s">
+        <v>105</v>
+      </c>
+      <c r="K8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="I9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="I11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="I12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="I14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="19"/>
+      <c r="I16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>1</v>
+      </c>
+      <c r="D18" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>2</v>
+      </c>
+      <c r="E18" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>4</v>
+      </c>
+      <c r="F18" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>6</v>
+      </c>
+      <c r="G18" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>12</v>
+      </c>
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>1.25</v>
+      </c>
+      <c r="D19" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>3</v>
+      </c>
+      <c r="E19" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>5</v>
+      </c>
+      <c r="F19" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>8</v>
+      </c>
+      <c r="G19" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>1.5</v>
+      </c>
+      <c r="D20" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>6</v>
+      </c>
+      <c r="F20" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>9</v>
+      </c>
+      <c r="G20" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>1.75</v>
+      </c>
+      <c r="D21" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>4</v>
+      </c>
+      <c r="E21" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>7</v>
+      </c>
+      <c r="F21" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>11</v>
+      </c>
+      <c r="G21" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>21</v>
+      </c>
+      <c r="I21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>4</v>
+      </c>
+      <c r="E22" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>8</v>
+      </c>
+      <c r="F22" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>12</v>
+      </c>
+      <c r="G22" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>24</v>
+      </c>
+      <c r="I22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>2.25</v>
+      </c>
+      <c r="D23" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>5</v>
+      </c>
+      <c r="E23" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>9</v>
+      </c>
+      <c r="F23" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>14</v>
+      </c>
+      <c r="G23" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>27</v>
+      </c>
+      <c r="I23" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>2.5</v>
+      </c>
+      <c r="D24" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>10</v>
+      </c>
+      <c r="F24" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>15</v>
+      </c>
+      <c r="G24" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>30</v>
+      </c>
+      <c r="I24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>2.75</v>
+      </c>
+      <c r="D25" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>11</v>
+      </c>
+      <c r="F25" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>17</v>
+      </c>
+      <c r="G25" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>33</v>
+      </c>
+      <c r="I25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>12</v>
+      </c>
+      <c r="F26" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>18</v>
+      </c>
+      <c r="G26" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>36</v>
+      </c>
+      <c r="I26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>3.25</v>
+      </c>
+      <c r="D27" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>7</v>
+      </c>
+      <c r="E27" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>13</v>
+      </c>
+      <c r="F27" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>20</v>
+      </c>
+      <c r="G27" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>39</v>
+      </c>
+      <c r="I27" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>3.5</v>
+      </c>
+      <c r="D28" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>7</v>
+      </c>
+      <c r="E28" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>14</v>
+      </c>
+      <c r="F28" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>21</v>
+      </c>
+      <c r="G28" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>42</v>
+      </c>
+      <c r="I28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>3.75</v>
+      </c>
+      <c r="D29" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>8</v>
+      </c>
+      <c r="E29" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>15</v>
+      </c>
+      <c r="F29" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>23</v>
+      </c>
+      <c r="G29" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>4</v>
+      </c>
+      <c r="D30" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>8</v>
+      </c>
+      <c r="E30" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>16</v>
+      </c>
+      <c r="F30" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>24</v>
+      </c>
+      <c r="G30" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>4.25</v>
+      </c>
+      <c r="D31" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>9</v>
+      </c>
+      <c r="E31" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>17</v>
+      </c>
+      <c r="F31" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>26</v>
+      </c>
+      <c r="G31" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>15</v>
+      </c>
+      <c r="C32">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>4.5</v>
+      </c>
+      <c r="D32" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>9</v>
+      </c>
+      <c r="E32" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>18</v>
+      </c>
+      <c r="F32" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>27</v>
+      </c>
+      <c r="G32" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>4.75</v>
+      </c>
+      <c r="D33" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>10</v>
+      </c>
+      <c r="E33" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>19</v>
+      </c>
+      <c r="F33" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>29</v>
+      </c>
+      <c r="G33" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>17</v>
+      </c>
+      <c r="C34">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>5</v>
+      </c>
+      <c r="D34" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>10</v>
+      </c>
+      <c r="E34" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>20</v>
+      </c>
+      <c r="F34" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>30</v>
+      </c>
+      <c r="G34" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>18</v>
+      </c>
+      <c r="C35">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>5.25</v>
+      </c>
+      <c r="D35" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>11</v>
+      </c>
+      <c r="E35" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>21</v>
+      </c>
+      <c r="F35" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>32</v>
+      </c>
+      <c r="G35" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>5.5</v>
+      </c>
+      <c r="D36" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>11</v>
+      </c>
+      <c r="E36" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>22</v>
+      </c>
+      <c r="F36" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>33</v>
+      </c>
+      <c r="G36" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <f>1+(Tableau7[[#This Row],[Level]]-1)*0.25</f>
+        <v>5.75</v>
+      </c>
+      <c r="D37" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</f>
+        <v>12</v>
+      </c>
+      <c r="E37" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</f>
+        <v>23</v>
+      </c>
+      <c r="F37" s="2">
+        <f>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</f>
+        <v>35</v>
+      </c>
+      <c r="G37" s="2">
+        <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D16:G16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="3">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6808,15 +8643,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6841,18 +8688,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enemy | modify | rebalance enemy with stage 1 = 0.5 to stage 100 = 1 with max 1.25
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Y0652097\Desktop\CESIproject\PythonProject\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB3D72F0-9722-446D-A4D3-E1A2C3BDF91A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403A4C3F-768B-48A1-8030-D83A369EDB97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evolutions" sheetId="1" r:id="rId1"/>
@@ -446,6 +446,34 @@
   </cellStyles>
   <dxfs count="26">
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -481,34 +509,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -792,24 +792,24 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Cause" dataDxfId="13"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Etat" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date report" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Date closure" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{B7D86D81-AA7C-449F-B13F-BFD0639F6955}" name="Commentary" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau2" displayName="Tableau2" ref="B2:D32" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="B2:D32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="LVL" dataDxfId="7">
       <calculatedColumnFormula>B2+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Xp avant le niveau suivant" dataDxfId="6">
       <calculatedColumnFormula>$C$3+B2*10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="XP depuis le début du jeu" dataDxfId="5">
       <calculatedColumnFormula>C3+D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -818,12 +818,12 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau3" displayName="Tableau3" ref="H2:J3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="H2:J3" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="2">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="lvl actuelle" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="xp actuelle" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="up ou pas ?" dataDxfId="0">
       <calculatedColumnFormula>IF(Tableau3[xp actuelle]&gt;=100+10*(Tableau3[lvl actuelle]-1),"Oui","Non")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1130,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:M29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1181,10 +1181,14 @@
         <v>1</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="F3" s="7">
+        <v>43865</v>
+      </c>
+      <c r="G3" s="7">
+        <v>43868</v>
+      </c>
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1287,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F8" s="7">
         <v>43864</v>
@@ -1306,10 +1310,14 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="F9" s="7">
+        <v>43871</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43871</v>
+      </c>
       <c r="H9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1679,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
@@ -6592,9 +6600,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6801,27 +6812,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6846,9 +6845,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="ab1f00cb-b678-48f7-aded-930f239c9527"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Weapon generation | Add | base of generation the carac generation, calculating the algorithme for numberDice and damage
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F90567-E560-4FF3-A3DB-537106B6B059}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B49D30-2CF4-4D57-B156-872DF15651AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="142">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -448,12 +448,27 @@
   </si>
   <si>
     <t>agility</t>
+  </si>
+  <si>
+    <t>OneHanded</t>
+  </si>
+  <si>
+    <t>Two handed</t>
+  </si>
+  <si>
+    <t>Two Weapon</t>
+  </si>
+  <si>
+    <t>Sword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0\D"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
@@ -515,7 +530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -523,11 +538,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -578,12 +621,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,6 +657,7 @@
   <dxfs count="31">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -607,7 +673,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1022,19 +1087,19 @@
   <autoFilter ref="B17:G37" xr:uid="{C892CB3D-BF9B-46E5-9300-BEA3BBCAEF09}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{A891AB08-64A9-4A19-B103-7079E9CB00C2}" name="Level"/>
-    <tableColumn id="5" xr3:uid="{8E2D95A1-93C7-4BF2-9825-41B55E7894BB}" name="Multiplicateur" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{8E2D95A1-93C7-4BF2-9825-41B55E7894BB}" name="Multiplicateur" dataDxfId="4">
       <calculatedColumnFormula>1+(Tableau7[[#This Row],[Level]]-1)*0.25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{BD052409-7DF4-4016-8B8D-C52FEE20CEC8}" name="Common" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{BD052409-7DF4-4016-8B8D-C52FEE20CEC8}" name="Common" dataDxfId="3">
       <calculatedColumnFormula>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Common",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{A15D3612-F474-4B9C-8C65-2BB0FE5F4915}" name="Rare" dataDxfId="3">
+    <tableColumn id="6" xr3:uid="{A15D3612-F474-4B9C-8C65-2BB0FE5F4915}" name="Rare" dataDxfId="2">
       <calculatedColumnFormula>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Rare",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3C43E1AB-E1B8-4592-B084-1B3D381FC6B2}" name="Epic" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{3C43E1AB-E1B8-4592-B084-1B3D381FC6B2}" name="Epic" dataDxfId="1">
       <calculatedColumnFormula>ROUNDUP(Tableau7[Multiplicateur]*VLOOKUP("Epic",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{B515297F-08B2-4D2C-B3D3-43FD65399196}" name="Legendary" dataDxfId="1">
+    <tableColumn id="8" xr3:uid="{B515297F-08B2-4D2C-B3D3-43FD65399196}" name="Legendary" dataDxfId="0">
       <calculatedColumnFormula>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -7338,7 +7403,7 @@
         <v>65</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68:C131" si="1">ROUNDDOWN(B68/4,0)+1</f>
+        <f t="shared" ref="C68:C103" si="1">ROUNDDOWN(B68/4,0)+1</f>
         <v>17</v>
       </c>
     </row>
@@ -7664,10 +7729,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:V37"/>
+  <dimension ref="B2:BK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7675,195 +7740,1575 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="21" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="29" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="40" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="E2" s="20"/>
+      <c r="I2" s="30">
+        <v>1</v>
+      </c>
+      <c r="J2" s="30">
+        <v>2</v>
+      </c>
+      <c r="K2" s="30">
+        <v>3</v>
+      </c>
+      <c r="L2" s="30">
+        <v>4</v>
+      </c>
+      <c r="M2" s="24"/>
+      <c r="P2" s="26">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="26">
+        <v>6</v>
+      </c>
+      <c r="R2" s="26">
+        <v>8</v>
+      </c>
+      <c r="S2" s="26">
+        <v>10</v>
+      </c>
+      <c r="T2" s="26">
+        <v>12</v>
+      </c>
+      <c r="U2" s="26">
+        <v>20</v>
+      </c>
+      <c r="V2" s="26">
+        <v>100</v>
+      </c>
+      <c r="W2" s="24"/>
+      <c r="Z2" s="26">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="26">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="26">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="26">
+        <v>4</v>
+      </c>
+      <c r="AH2" s="26">
+        <v>4</v>
+      </c>
+      <c r="AI2" s="26">
+        <v>6</v>
+      </c>
+      <c r="AJ2" s="26">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="26">
+        <v>10</v>
+      </c>
+      <c r="AL2" s="26">
+        <v>12</v>
+      </c>
+      <c r="AM2" s="26">
+        <v>20</v>
+      </c>
+      <c r="AN2" s="26">
+        <v>100</v>
+      </c>
+      <c r="AO2" s="24"/>
+    </row>
+    <row r="3" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>89</v>
       </c>
       <c r="C3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="26">
+        <v>80</v>
+      </c>
+      <c r="J3" s="26">
+        <v>19</v>
+      </c>
+      <c r="K3" s="26">
+        <v>1</v>
+      </c>
+      <c r="L3" s="26">
+        <v>0</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="N3">
+        <f>($I$2*I3+$J$2*J3+$K$2*K3+$L$2*L3)/SUM(I3:L3)</f>
+        <v>1.21</v>
+      </c>
+      <c r="P3" s="26">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="26">
+        <v>25</v>
+      </c>
+      <c r="R3" s="26">
+        <v>10</v>
+      </c>
+      <c r="S3" s="26">
+        <v>5</v>
+      </c>
+      <c r="T3" s="26">
+        <v>0</v>
+      </c>
+      <c r="U3" s="26">
+        <v>0</v>
+      </c>
+      <c r="V3" s="26">
+        <v>0</v>
+      </c>
+      <c r="W3" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="X3">
+        <f>(P3*$P$2+Q3*$Q$2+R3*$R$2+S3*$S$2+T3*$T$2+U3*$U$2+V3*$V$2)/SUM(P3:V3)</f>
+        <v>5.2</v>
+      </c>
+      <c r="Z3" s="29">
+        <f>I9/200+I3/200</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="AA3" s="29">
+        <f t="shared" ref="AA3:AC3" si="0">J9/200+J3/200</f>
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="AB3" s="29">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AC3" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE3" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF3">
+        <f>($Z$2*Z3+$AA$2*AA3+$AB$2*AB3+$AC$2*AC3)/SUM(Z3:AC3)</f>
+        <v>1.155</v>
+      </c>
+      <c r="AH3" s="29">
+        <f>P3/200+P11/200</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="AI3" s="29">
+        <f>Q3/200+Q11/200</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AJ3" s="29">
+        <f>R3/200+R11/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AK3" s="29">
+        <f>S3/200+S11/200</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="AL3" s="29">
+        <f>T3/200+T11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AM3" s="29">
+        <f>U3/200+U11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AN3" s="29">
+        <f>V3/200+V11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO3" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP3" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ3">
+        <f>($AH$2*AH3+$AI$2*AI3+$AJ$2*AJ3+$AK$2*AK3+$AL$2*AL3+$AM$2*AM3+$AN$2*AN3)/SUM(AH3:AN3)</f>
+        <v>5.5299999999999994</v>
+      </c>
+      <c r="BI3" t="s">
         <v>102</v>
       </c>
-      <c r="K3" t="s">
+      <c r="BK3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>90</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="26">
+        <v>70</v>
+      </c>
+      <c r="J4" s="26">
+        <v>28</v>
+      </c>
+      <c r="K4" s="26">
+        <v>2</v>
+      </c>
+      <c r="L4" s="26">
+        <v>0</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N6" si="1">($I$2*I4+$J$2*J4+$K$2*K4+$L$2*L4)/SUM(I4:L4)</f>
+        <v>1.32</v>
+      </c>
+      <c r="P4" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="26">
+        <v>20</v>
+      </c>
+      <c r="R4" s="26">
+        <v>50</v>
+      </c>
+      <c r="S4" s="26">
+        <v>20</v>
+      </c>
+      <c r="T4" s="26">
+        <v>9</v>
+      </c>
+      <c r="U4" s="26">
+        <v>1</v>
+      </c>
+      <c r="V4" s="26">
+        <v>0</v>
+      </c>
+      <c r="W4" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ref="X4:X8" si="2">(P4*$P$2+Q4*$Q$2+R4*$R$2+S4*$S$2+T4*$T$2+U4*$U$2+V4*$V$2)/SUM(P4:V4)</f>
+        <v>8.48</v>
+      </c>
+      <c r="Z4" s="29">
+        <f>I9/200+I4/200</f>
+        <v>0.8</v>
+      </c>
+      <c r="AA4" s="29">
+        <f t="shared" ref="AA4:AC4" si="3">J9/200+J4/200</f>
+        <v>0.19</v>
+      </c>
+      <c r="AB4" s="29">
+        <f t="shared" si="3"/>
+        <v>0.01</v>
+      </c>
+      <c r="AC4" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" ref="AF4:AF14" si="4">($Z$2*Z4+$AA$2*AA4+$AB$2*AB4+$AC$2*AC4)/SUM(Z4:AC4)</f>
+        <v>1.2100000000000002</v>
+      </c>
+      <c r="AH4" s="29">
+        <f>P3/200+P12/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AI4" s="29">
+        <f>Q3/200+Q12/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AJ4" s="29">
+        <f>R3/200+R12/200</f>
+        <v>0.32</v>
+      </c>
+      <c r="AK4" s="29">
+        <f>S3/200+S12/200</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="AL4" s="29">
+        <f>T3/200+T12/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AM4" s="29">
+        <f>U3/200+U12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AN4" s="29">
+        <f>V3/200+V12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO4" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP4" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ4">
+        <f t="shared" ref="AQ4:AQ26" si="5">($AH$2*AH4+$AI$2*AI4+$AJ$2*AJ4+$AK$2*AK4+$AL$2*AL4+$AM$2*AM4+$AN$2*AN4)/SUM(AH4:AN4)</f>
+        <v>6.370000000000001</v>
+      </c>
+      <c r="BI4" t="s">
         <v>109</v>
       </c>
-      <c r="K4" t="s">
+      <c r="BK4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>91</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="26">
+        <v>50</v>
+      </c>
+      <c r="J5" s="26">
+        <v>39</v>
+      </c>
+      <c r="K5" s="26">
+        <v>10</v>
+      </c>
+      <c r="L5" s="26">
+        <v>1</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>1.62</v>
+      </c>
+      <c r="P5" s="26">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="26">
+        <v>25</v>
+      </c>
+      <c r="R5" s="26">
+        <v>35</v>
+      </c>
+      <c r="S5" s="26">
+        <v>25</v>
+      </c>
+      <c r="T5" s="26">
+        <v>9</v>
+      </c>
+      <c r="U5" s="26">
+        <v>1</v>
+      </c>
+      <c r="V5" s="26">
+        <v>0</v>
+      </c>
+      <c r="W5" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="2"/>
+        <v>8.2799999999999994</v>
+      </c>
+      <c r="Z5" s="29">
+        <f>I9/200+I5/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="AA5" s="29">
+        <f t="shared" ref="AA5:AC5" si="6">J9/200+J5/200</f>
+        <v>0.245</v>
+      </c>
+      <c r="AB5" s="29">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="AC5" s="29">
+        <f t="shared" si="6"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AD5" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE5" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="4"/>
+        <v>1.3599999999999999</v>
+      </c>
+      <c r="AH5" s="29">
+        <f>P3/200+P13/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AI5" s="29">
+        <f>Q3/200+Q13/200</f>
+        <v>0.125</v>
+      </c>
+      <c r="AJ5" s="29">
+        <f>R3/200+R13/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AK5" s="29">
+        <f>S3/200+S13/200</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="AL5" s="29">
+        <f>T3/200+T13/200</f>
+        <v>0.05</v>
+      </c>
+      <c r="AM5" s="29">
+        <f>U3/200+U13/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AN5" s="29">
+        <f>V3/200+V13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO5" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="K5" t="s">
+      <c r="AP5" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ5">
+        <f t="shared" si="5"/>
+        <v>7.4499999999999993</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BK5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>92</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="26">
+        <v>0</v>
+      </c>
+      <c r="J6" s="26">
+        <v>60</v>
+      </c>
+      <c r="K6" s="26">
+        <v>30</v>
+      </c>
+      <c r="L6" s="26">
+        <v>10</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="P6" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="26">
+        <v>0</v>
+      </c>
+      <c r="R6" s="26">
+        <v>20</v>
+      </c>
+      <c r="S6" s="26">
+        <v>60</v>
+      </c>
+      <c r="T6" s="26">
+        <v>18</v>
+      </c>
+      <c r="U6" s="26">
+        <v>2</v>
+      </c>
+      <c r="V6" s="26">
+        <v>0</v>
+      </c>
+      <c r="W6" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>10.16</v>
+      </c>
+      <c r="Z6" s="29">
+        <f>I9/200+I6/200</f>
+        <v>0.45</v>
+      </c>
+      <c r="AA6" s="29">
+        <f t="shared" ref="AA6:AC6" si="7">J9/200+J6/200</f>
+        <v>0.35</v>
+      </c>
+      <c r="AB6" s="29">
+        <f t="shared" si="7"/>
+        <v>0.15</v>
+      </c>
+      <c r="AC6" s="29">
+        <f t="shared" si="7"/>
+        <v>0.05</v>
+      </c>
+      <c r="AD6" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="4"/>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="AH6" s="29">
+        <f>P3/200+P14/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AI6" s="29">
+        <f>Q3/200+Q14/200</f>
+        <v>0.125</v>
+      </c>
+      <c r="AJ6" s="29">
+        <f>R3/200+R14/200</f>
+        <v>0.05</v>
+      </c>
+      <c r="AK6" s="29">
+        <f>S3/200+S14/200</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AL6" s="29">
+        <f>T3/200+T14/200</f>
+        <v>0.15</v>
+      </c>
+      <c r="AM6" s="29">
+        <f>U3/200+U14/200</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AN6" s="29">
+        <f>V3/200+V14/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO6" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP6" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ6">
+        <f t="shared" si="5"/>
+        <v>9.2999999999999989</v>
+      </c>
+      <c r="BI6" t="s">
         <v>104</v>
       </c>
-      <c r="K6" t="s">
+      <c r="BK6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>93</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="I7" t="s">
+      <c r="E7" s="20"/>
+      <c r="P7" s="26">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="26">
+        <v>30</v>
+      </c>
+      <c r="R7" s="26">
+        <v>35</v>
+      </c>
+      <c r="S7" s="26">
+        <v>10</v>
+      </c>
+      <c r="T7" s="26">
+        <v>8</v>
+      </c>
+      <c r="U7" s="26">
+        <v>2</v>
+      </c>
+      <c r="V7" s="26">
+        <v>0</v>
+      </c>
+      <c r="W7" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>7.56</v>
+      </c>
+      <c r="Z7" s="29">
+        <f>I10/200+I3/200</f>
+        <v>0.44</v>
+      </c>
+      <c r="AA7" s="29">
+        <f t="shared" ref="AA7:AC7" si="8">J10/200+J3/200</f>
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="AB7" s="29">
+        <f t="shared" si="8"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AC7" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AD7" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF7">
+        <f t="shared" si="4"/>
+        <v>1.575</v>
+      </c>
+      <c r="AH7" s="29">
+        <f>P$4/200+P11/200</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AI7" s="29">
+        <f>Q$4/200+Q11/200</f>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="AJ7" s="29">
+        <f>R$4/200+R11/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AK7" s="29">
+        <f>S$4/200+S11/200</f>
+        <v>0.10500000000000001</v>
+      </c>
+      <c r="AL7" s="29">
+        <f>T$4/200+T11/200</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AM7" s="29">
+        <f>U$4/200+U11/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN7" s="29">
+        <f>V$4/200+V11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO7" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP7" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ7">
+        <f t="shared" si="5"/>
+        <v>7.169999999999999</v>
+      </c>
+      <c r="BI7" t="s">
         <v>106</v>
       </c>
-      <c r="K7" t="s">
+      <c r="BK7" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="E8" s="21"/>
-      <c r="I8" t="s">
+    <row r="8" spans="2:63" x14ac:dyDescent="0.2">
+      <c r="E8" s="20"/>
+      <c r="I8" s="30">
+        <v>1</v>
+      </c>
+      <c r="J8" s="30">
+        <v>2</v>
+      </c>
+      <c r="K8" s="30">
+        <v>3</v>
+      </c>
+      <c r="L8" s="30">
+        <v>4</v>
+      </c>
+      <c r="M8" s="24"/>
+      <c r="P8" s="26">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="26">
+        <v>35</v>
+      </c>
+      <c r="R8" s="26">
+        <v>25</v>
+      </c>
+      <c r="S8" s="26">
+        <v>10</v>
+      </c>
+      <c r="T8" s="26">
+        <v>7</v>
+      </c>
+      <c r="U8" s="26">
+        <v>3</v>
+      </c>
+      <c r="V8" s="26">
+        <v>0</v>
+      </c>
+      <c r="W8" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>7.34</v>
+      </c>
+      <c r="Z8" s="29">
+        <f>I10/200+I4/200</f>
+        <v>0.38999999999999996</v>
+      </c>
+      <c r="AA8" s="29">
+        <f t="shared" ref="AA8:AC8" si="9">J10/200+J4/200</f>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="AB8" s="29">
+        <f t="shared" si="9"/>
+        <v>0.02</v>
+      </c>
+      <c r="AC8" s="29">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="4"/>
+        <v>1.6300000000000001</v>
+      </c>
+      <c r="AH8" s="29">
+        <f>P$4/200+P12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="29">
+        <f>Q$4/200+Q12/200</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AJ8" s="29">
+        <f>R$4/200+R12/200</f>
+        <v>0.52</v>
+      </c>
+      <c r="AK8" s="29">
+        <f>S$4/200+S12/200</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL8" s="29">
+        <f>T$4/200+T12/200</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="AM8" s="29">
+        <f>U$4/200+U12/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN8" s="29">
+        <f>V$4/200+V12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO8" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ8">
+        <f t="shared" si="5"/>
+        <v>8.01</v>
+      </c>
+      <c r="BI8" t="s">
         <v>105</v>
       </c>
-      <c r="K8" t="s">
+      <c r="BK8" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="I9" t="s">
+      <c r="E9" s="20"/>
+      <c r="I9" s="26">
+        <v>90</v>
+      </c>
+      <c r="J9" s="26">
+        <v>10</v>
+      </c>
+      <c r="K9" s="26">
+        <v>0</v>
+      </c>
+      <c r="L9" s="26">
+        <v>0</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="N9">
+        <f>($I$2*I9+$J$2*J9+$K$2*K9+$L$2*L9)/SUM(I9:L9)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Z9" s="29">
+        <f>I10/200+I5/200</f>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AA9" s="29">
+        <f t="shared" ref="AA9:AC9" si="10">J10/200+J5/200</f>
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="AB9" s="29">
+        <f t="shared" si="10"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="AC9" s="29">
+        <f t="shared" si="10"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AD9" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE9" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="4"/>
+        <v>1.78</v>
+      </c>
+      <c r="AH9" s="29">
+        <f>P$4/200+P13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AI9" s="29">
+        <f>Q$4/200+Q13/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AJ9" s="29">
+        <f>R$4/200+R13/200</f>
+        <v>0.5</v>
+      </c>
+      <c r="AK9" s="29">
+        <f>S$4/200+S13/200</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="AL9" s="29">
+        <f>T$4/200+T13/200</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AM9" s="29">
+        <f>U$4/200+U13/200</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="AN9" s="29">
+        <f>V$4/200+V13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO9" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP9" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ9">
+        <f t="shared" si="5"/>
+        <v>9.09</v>
+      </c>
+      <c r="BI9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="I10" t="s">
+      <c r="E10" s="20"/>
+      <c r="I10" s="26">
+        <v>8</v>
+      </c>
+      <c r="J10" s="26">
+        <v>90</v>
+      </c>
+      <c r="K10" s="26">
+        <v>2</v>
+      </c>
+      <c r="L10" s="26">
+        <v>0</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10:N12" si="11">($I$2*I10+$J$2*J10+$K$2*K10+$L$2*L10)/SUM(I10:L10)</f>
+        <v>1.94</v>
+      </c>
+      <c r="P10" s="26">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="26">
+        <v>6</v>
+      </c>
+      <c r="R10" s="26">
+        <v>8</v>
+      </c>
+      <c r="S10" s="26">
+        <v>10</v>
+      </c>
+      <c r="T10" s="26">
+        <v>12</v>
+      </c>
+      <c r="U10" s="26">
+        <v>20</v>
+      </c>
+      <c r="V10" s="26">
+        <v>100</v>
+      </c>
+      <c r="Z10" s="29">
+        <f>I10/200+I6/200</f>
+        <v>0.04</v>
+      </c>
+      <c r="AA10" s="29">
+        <f t="shared" ref="AA10:AC10" si="12">J10/200+J6/200</f>
+        <v>0.75</v>
+      </c>
+      <c r="AB10" s="29">
+        <f t="shared" si="12"/>
+        <v>0.16</v>
+      </c>
+      <c r="AC10" s="29">
+        <f t="shared" si="12"/>
+        <v>0.05</v>
+      </c>
+      <c r="AD10" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE10" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="4"/>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AH10" s="29">
+        <f>P$4/200+P14/200</f>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="29">
+        <f>Q$4/200+Q14/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AJ10" s="29">
+        <f>R$4/200+R14/200</f>
+        <v>0.25</v>
+      </c>
+      <c r="AK10" s="29">
+        <f>S$4/200+S14/200</f>
+        <v>0.35</v>
+      </c>
+      <c r="AL10" s="29">
+        <f>T$4/200+T14/200</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AM10" s="29">
+        <f>U$4/200+U14/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AN10" s="29">
+        <f>V$4/200+V14/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO10" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP10" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ10">
+        <f t="shared" si="5"/>
+        <v>10.94</v>
+      </c>
+      <c r="BI10" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>90</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="I11" t="s">
+      <c r="E11" s="20"/>
+      <c r="I11" s="26">
+        <v>60</v>
+      </c>
+      <c r="J11" s="26">
+        <v>35</v>
+      </c>
+      <c r="K11" s="26">
+        <v>5</v>
+      </c>
+      <c r="L11" s="26">
+        <v>0</v>
+      </c>
+      <c r="M11" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="11"/>
+        <v>1.45</v>
+      </c>
+      <c r="P11" s="26">
+        <v>19</v>
+      </c>
+      <c r="Q11" s="26">
+        <v>70</v>
+      </c>
+      <c r="R11" s="26">
+        <v>10</v>
+      </c>
+      <c r="S11" s="26">
+        <v>1</v>
+      </c>
+      <c r="T11" s="26">
+        <v>0</v>
+      </c>
+      <c r="U11" s="26">
+        <v>0</v>
+      </c>
+      <c r="V11" s="26">
+        <v>0</v>
+      </c>
+      <c r="W11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="X11">
+        <f>(P11*$P$2+Q11*$Q$2+R11*$R$2+S11*$S$2+T11*$T$2+U11*$U$2+V11*$V$2)/SUM(P11:V11)</f>
+        <v>5.86</v>
+      </c>
+      <c r="Z11" s="29">
+        <f>I11/200+I3/200</f>
+        <v>0.7</v>
+      </c>
+      <c r="AA11" s="29">
+        <f t="shared" ref="AA11:AC11" si="13">J11/200+J3/200</f>
+        <v>0.27</v>
+      </c>
+      <c r="AB11" s="29">
+        <f t="shared" si="13"/>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="AC11" s="29">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="4"/>
+        <v>1.33</v>
+      </c>
+      <c r="AH11" s="29">
+        <f>P$5/200+P11/200</f>
+        <v>0.12</v>
+      </c>
+      <c r="AI11" s="29">
+        <f>Q$5/200+Q11/200</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AJ11" s="29">
+        <f>R$5/200+R11/200</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="AK11" s="29">
+        <f>S$5/200+S11/200</f>
+        <v>0.13</v>
+      </c>
+      <c r="AL11" s="29">
+        <f>T$5/200+T11/200</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AM11" s="29">
+        <f>U$5/200+U11/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN11" s="29">
+        <f>V$5/200+V11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP11" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ11">
+        <f t="shared" si="5"/>
+        <v>7.0699999999999985</v>
+      </c>
+      <c r="BI11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>91</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="25"/>
+      <c r="P12" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="26">
+        <v>35</v>
+      </c>
+      <c r="R12" s="26">
+        <v>54</v>
+      </c>
+      <c r="S12" s="26">
+        <v>10</v>
+      </c>
+      <c r="T12" s="26">
+        <v>1</v>
+      </c>
+      <c r="U12" s="26">
+        <v>0</v>
+      </c>
+      <c r="V12" s="26">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="X12">
+        <f t="shared" ref="X12:X14" si="14">(P12*$P$2+Q12*$Q$2+R12*$R$2+S12*$S$2+T12*$T$2+U12*$U$2+V12*$V$2)/SUM(P12:V12)</f>
+        <v>7.54</v>
+      </c>
+      <c r="Z12" s="29">
+        <f>I11/200+I4/200</f>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="AA12" s="29">
+        <f t="shared" ref="AA12:AC12" si="15">J11/200+J4/200</f>
+        <v>0.315</v>
+      </c>
+      <c r="AB12" s="29">
+        <f t="shared" si="15"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC12" s="29">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF12">
+        <f t="shared" si="4"/>
+        <v>1.385</v>
+      </c>
+      <c r="AH12" s="29">
+        <f>P$5/200+P12/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AI12" s="29">
+        <f>Q$5/200+Q12/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AJ12" s="29">
+        <f>R$5/200+R12/200</f>
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="AK12" s="29">
+        <f>S$5/200+S12/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AL12" s="29">
+        <f>T$5/200+T12/200</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="AM12" s="29">
+        <f>U$5/200+U12/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN12" s="29">
+        <f>V$5/200+V12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO12" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP12" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ12">
+        <f t="shared" si="5"/>
+        <v>7.9099999999999993</v>
+      </c>
+      <c r="BI12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>92</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="I13" t="s">
+      <c r="P13" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="26">
+        <v>0</v>
+      </c>
+      <c r="R13" s="26">
+        <v>50</v>
+      </c>
+      <c r="S13" s="26">
+        <v>35</v>
+      </c>
+      <c r="T13" s="26">
+        <v>10</v>
+      </c>
+      <c r="U13" s="26">
+        <v>5</v>
+      </c>
+      <c r="V13" s="26">
+        <v>0</v>
+      </c>
+      <c r="W13" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="14"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="Z13" s="29">
+        <f>I11/200+I5/200</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AA13" s="29">
+        <f t="shared" ref="AA13:AC13" si="16">J11/200+J5/200</f>
+        <v>0.37</v>
+      </c>
+      <c r="AB13" s="29">
+        <f t="shared" si="16"/>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="AC13" s="29">
+        <f t="shared" si="16"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AD13" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE13" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF13">
+        <f t="shared" si="4"/>
+        <v>1.5350000000000001</v>
+      </c>
+      <c r="AH13" s="29">
+        <f>P$5/200+P13/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AI13" s="29">
+        <f>Q$5/200+Q13/200</f>
+        <v>0.125</v>
+      </c>
+      <c r="AJ13" s="29">
+        <f>R$5/200+R13/200</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="AK13" s="29">
+        <f>S$5/200+S13/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AL13" s="29">
+        <f>T$5/200+T13/200</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AM13" s="29">
+        <f>U$5/200+U13/200</f>
+        <v>3.0000000000000002E-2</v>
+      </c>
+      <c r="AN13" s="29">
+        <f>V$5/200+V13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO13" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP13" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ13">
+        <f t="shared" si="5"/>
+        <v>8.99</v>
+      </c>
+      <c r="BI13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>99</v>
       </c>
       <c r="C14">
         <v>12</v>
       </c>
-      <c r="I14" t="s">
+      <c r="P14" s="26">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="26">
+        <v>0</v>
+      </c>
+      <c r="R14" s="26">
+        <v>0</v>
+      </c>
+      <c r="S14" s="26">
+        <v>50</v>
+      </c>
+      <c r="T14" s="26">
+        <v>30</v>
+      </c>
+      <c r="U14" s="26">
+        <v>19</v>
+      </c>
+      <c r="V14" s="26">
+        <v>1</v>
+      </c>
+      <c r="W14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="14"/>
+        <v>13.4</v>
+      </c>
+      <c r="Z14" s="29">
+        <f>I11/200+I6/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AA14" s="29">
+        <f t="shared" ref="AA14:AC14" si="17">J11/200+J6/200</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AB14" s="29">
+        <f t="shared" si="17"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AC14" s="29">
+        <f t="shared" si="17"/>
+        <v>0.05</v>
+      </c>
+      <c r="AD14" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF14">
+        <f t="shared" si="4"/>
+        <v>1.9749999999999999</v>
+      </c>
+      <c r="AH14" s="29">
+        <f>P$5/200+P14/200</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AI14" s="29">
+        <f>Q$5/200+Q14/200</f>
+        <v>0.125</v>
+      </c>
+      <c r="AJ14" s="29">
+        <f>R$5/200+R14/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AK14" s="29">
+        <f>S$5/200+S14/200</f>
+        <v>0.375</v>
+      </c>
+      <c r="AL14" s="29">
+        <f>T$5/200+T14/200</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AM14" s="29">
+        <f>U$5/200+U14/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AN14" s="29">
+        <f>V$5/200+V14/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO14" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP14" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ14">
+        <f t="shared" si="5"/>
+        <v>10.84</v>
+      </c>
+      <c r="BI14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="I15" t="s">
+    <row r="15" spans="2:63" x14ac:dyDescent="0.2">
+      <c r="AH15" s="29">
+        <f>P$6/200+P11/200</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AI15" s="29">
+        <f>Q$6/200+Q11/200</f>
+        <v>0.35</v>
+      </c>
+      <c r="AJ15" s="29">
+        <f>R$6/200+R11/200</f>
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AK15" s="29">
+        <f>S$6/200+S11/200</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="AL15" s="29">
+        <f>T$6/200+T11/200</f>
+        <v>0.09</v>
+      </c>
+      <c r="AM15" s="29">
+        <f>U$6/200+U11/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="AN15" s="29">
+        <f>V$6/200+V11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO15" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP15" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ15">
+        <f t="shared" si="5"/>
+        <v>8.0100000000000016</v>
+      </c>
+      <c r="BI15" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D16" s="20" t="s">
+    <row r="16" spans="2:63" x14ac:dyDescent="0.2">
+      <c r="D16" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="19"/>
-      <c r="I16" t="s">
+      <c r="AH16" s="29">
+        <f>P$6/200+P12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AI16" s="29">
+        <f>Q$6/200+Q12/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AJ16" s="29">
+        <f>R$6/200+R12/200</f>
+        <v>0.37</v>
+      </c>
+      <c r="AK16" s="29">
+        <f>S$6/200+S12/200</f>
+        <v>0.35</v>
+      </c>
+      <c r="AL16" s="29">
+        <f>T$6/200+T12/200</f>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="AM16" s="29">
+        <f>U$6/200+U12/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="AN16" s="29">
+        <f>V$6/200+V12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO16" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP16" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ16">
+        <f t="shared" si="5"/>
+        <v>8.8500000000000014</v>
+      </c>
+      <c r="BI16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>97</v>
       </c>
@@ -7882,11 +9327,50 @@
       <c r="G17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I17" t="s">
+      <c r="O17" s="25"/>
+      <c r="AH17" s="29">
+        <f>P$6/200+P13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AI17" s="29">
+        <f>Q$6/200+Q13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="29">
+        <f>R$6/200+R13/200</f>
+        <v>0.35</v>
+      </c>
+      <c r="AK17" s="29">
+        <f>S$6/200+S13/200</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AL17" s="29">
+        <f>T$6/200+T13/200</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AM17" s="29">
+        <f>U$6/200+U13/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AN17" s="29">
+        <f>V$6/200+V13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO17" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP17" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ17">
+        <f t="shared" si="5"/>
+        <v>9.93</v>
+      </c>
+      <c r="BI17" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>1</v>
       </c>
@@ -7910,11 +9394,50 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>12</v>
       </c>
-      <c r="I18" t="s">
+      <c r="O18" s="25"/>
+      <c r="AH18" s="29">
+        <f>P$6/200+P14/200</f>
+        <v>0</v>
+      </c>
+      <c r="AI18" s="29">
+        <f>Q$6/200+Q14/200</f>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="29">
+        <f>R$6/200+R14/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AK18" s="29">
+        <f>S$6/200+S14/200</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AL18" s="29">
+        <f>T$6/200+T14/200</f>
+        <v>0.24</v>
+      </c>
+      <c r="AM18" s="29">
+        <f>U$6/200+U14/200</f>
+        <v>0.105</v>
+      </c>
+      <c r="AN18" s="29">
+        <f>V$6/200+V14/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO18" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP18" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" si="5"/>
+        <v>11.78</v>
+      </c>
+      <c r="BI18" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B19">
         <v>2</v>
       </c>
@@ -7938,11 +9461,50 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>15</v>
       </c>
-      <c r="I19" t="s">
+      <c r="O19" s="25"/>
+      <c r="AH19" s="29">
+        <f>P$7/200+P11/200</f>
+        <v>0.16999999999999998</v>
+      </c>
+      <c r="AI19" s="29">
+        <f>Q$7/200+Q11/200</f>
+        <v>0.5</v>
+      </c>
+      <c r="AJ19" s="29">
+        <f>R$7/200+R11/200</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="AK19" s="29">
+        <f>S$7/200+S11/200</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="AL19" s="29">
+        <f>T$7/200+T11/200</f>
+        <v>0.04</v>
+      </c>
+      <c r="AM19" s="29">
+        <f>U$7/200+U11/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="AN19" s="29">
+        <f>V$7/200+V11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO19" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP19" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ19">
+        <f t="shared" si="5"/>
+        <v>6.71</v>
+      </c>
+      <c r="BI19" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B20">
         <v>3</v>
       </c>
@@ -7966,11 +9528,50 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>18</v>
       </c>
-      <c r="I20" t="s">
+      <c r="O20" s="25"/>
+      <c r="AH20" s="29">
+        <f>P$7/200+P12/200</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AI20" s="29">
+        <f>Q$7/200+Q12/200</f>
+        <v>0.32499999999999996</v>
+      </c>
+      <c r="AJ20" s="29">
+        <f>R$7/200+R12/200</f>
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="AK20" s="29">
+        <f>S$7/200+S12/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AL20" s="29">
+        <f>T$7/200+T12/200</f>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AM20" s="29">
+        <f>U$7/200+U12/200</f>
+        <v>0.01</v>
+      </c>
+      <c r="AN20" s="29">
+        <f>V$7/200+V12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO20" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ20">
+        <f t="shared" si="5"/>
+        <v>7.55</v>
+      </c>
+      <c r="BI20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B21">
         <v>4</v>
       </c>
@@ -7994,11 +9595,49 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>21</v>
       </c>
-      <c r="I21" t="s">
+      <c r="AH21" s="29">
+        <f>P$7/200+P13/200</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AI21" s="29">
+        <f>Q$7/200+Q13/200</f>
+        <v>0.15</v>
+      </c>
+      <c r="AJ21" s="29">
+        <f>R$7/200+R13/200</f>
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="AK21" s="29">
+        <f>S$7/200+S13/200</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="AL21" s="29">
+        <f>T$7/200+T13/200</f>
+        <v>0.09</v>
+      </c>
+      <c r="AM21" s="29">
+        <f>U$7/200+U13/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AN21" s="29">
+        <f>V$7/200+V13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO21" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP21" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ21">
+        <f t="shared" si="5"/>
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="BI21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B22">
         <v>5</v>
       </c>
@@ -8022,11 +9661,49 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>24</v>
       </c>
-      <c r="I22" t="s">
+      <c r="AH22" s="29">
+        <f>P$7/200+P14/200</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AI22" s="29">
+        <f>Q$7/200+Q14/200</f>
+        <v>0.15</v>
+      </c>
+      <c r="AJ22" s="29">
+        <f>R$7/200+R14/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AK22" s="29">
+        <f>S$7/200+S14/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AL22" s="29">
+        <f>T$7/200+T14/200</f>
+        <v>0.19</v>
+      </c>
+      <c r="AM22" s="29">
+        <f>U$7/200+U14/200</f>
+        <v>0.105</v>
+      </c>
+      <c r="AN22" s="29">
+        <f>V$7/200+V14/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO22" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="AP22" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ22">
+        <f t="shared" si="5"/>
+        <v>10.480000000000002</v>
+      </c>
+      <c r="BI22" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B23">
         <v>6</v>
       </c>
@@ -8050,11 +9727,49 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>27</v>
       </c>
-      <c r="I23" t="s">
+      <c r="AH23" s="29">
+        <f>P$8/200+P11/200</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AI23" s="29">
+        <f>Q$8/200+Q11/200</f>
+        <v>0.52499999999999991</v>
+      </c>
+      <c r="AJ23" s="29">
+        <f>R$8/200+R11/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AK23" s="29">
+        <f>S$8/200+S11/200</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="AL23" s="29">
+        <f>T$8/200+T11/200</f>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AM23" s="29">
+        <f>U$8/200+U11/200</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AN23" s="29">
+        <f>V$8/200+V11/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO23" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AP23" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ23">
+        <f t="shared" si="5"/>
+        <v>6.6</v>
+      </c>
+      <c r="BI23" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>7</v>
       </c>
@@ -8078,11 +9793,49 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>30</v>
       </c>
-      <c r="I24" t="s">
+      <c r="AH24" s="29">
+        <f>P$8/200+P12/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AI24" s="29">
+        <f>Q$8/200+Q12/200</f>
+        <v>0.35</v>
+      </c>
+      <c r="AJ24" s="29">
+        <f>R$8/200+R12/200</f>
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="AK24" s="29">
+        <f>S$8/200+S12/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AL24" s="29">
+        <f>T$8/200+T12/200</f>
+        <v>0.04</v>
+      </c>
+      <c r="AM24" s="29">
+        <f>U$8/200+U12/200</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="AN24" s="29">
+        <f>V$8/200+V12/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AP24" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ24">
+        <f t="shared" si="5"/>
+        <v>7.44</v>
+      </c>
+      <c r="BI24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>8</v>
       </c>
@@ -8106,11 +9859,49 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>33</v>
       </c>
-      <c r="I25" t="s">
+      <c r="AH25" s="29">
+        <f>P$8/200+P13/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AI25" s="29">
+        <f>Q$8/200+Q13/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AJ25" s="29">
+        <f>R$8/200+R13/200</f>
+        <v>0.375</v>
+      </c>
+      <c r="AK25" s="29">
+        <f>S$8/200+S13/200</f>
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="AL25" s="29">
+        <f>T$8/200+T13/200</f>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AM25" s="29">
+        <f>U$8/200+U13/200</f>
+        <v>0.04</v>
+      </c>
+      <c r="AN25" s="29">
+        <f>V$8/200+V13/200</f>
+        <v>0</v>
+      </c>
+      <c r="AO25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AP25" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ25">
+        <f t="shared" si="5"/>
+        <v>8.52</v>
+      </c>
+      <c r="BI25" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>9</v>
       </c>
@@ -8134,11 +9925,49 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>36</v>
       </c>
-      <c r="I26" t="s">
+      <c r="AH26" s="29">
+        <f>P$8/200+P14/200</f>
+        <v>0.1</v>
+      </c>
+      <c r="AI26" s="29">
+        <f>Q$8/200+Q14/200</f>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="AJ26" s="29">
+        <f>R$8/200+R14/200</f>
+        <v>0.125</v>
+      </c>
+      <c r="AK26" s="29">
+        <f>S$8/200+S14/200</f>
+        <v>0.3</v>
+      </c>
+      <c r="AL26" s="29">
+        <f>T$8/200+T14/200</f>
+        <v>0.185</v>
+      </c>
+      <c r="AM26" s="29">
+        <f>U$8/200+U14/200</f>
+        <v>0.11</v>
+      </c>
+      <c r="AN26" s="29">
+        <f>V$8/200+V14/200</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO26" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AP26" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ26">
+        <f t="shared" si="5"/>
+        <v>10.37</v>
+      </c>
+      <c r="BI26" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>10</v>
       </c>
@@ -8162,11 +9991,11 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>39</v>
       </c>
-      <c r="I27" t="s">
+      <c r="BI27" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B28">
         <v>11</v>
       </c>
@@ -8190,11 +10019,11 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>42</v>
       </c>
-      <c r="I28" t="s">
+      <c r="BI28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B29">
         <v>12</v>
       </c>
@@ -8219,7 +10048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B30">
         <v>13</v>
       </c>
@@ -8244,7 +10073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B31">
         <v>14</v>
       </c>
@@ -8269,7 +10098,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:61" x14ac:dyDescent="0.2">
       <c r="B32">
         <v>15</v>
       </c>
@@ -8440,6 +10269,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D561B29C098A574288915AA7FDCE85A0" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="250102bec12d8b142e58c1d00b1ffd8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ee89e3b8-fbf6-4f90-a67d-b465f66f191f" xmlns:ns4="ab1f00cb-b678-48f7-aded-930f239c9527" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="440e872eed80589242d868d6c2b803d1" ns3:_="" ns4:_="">
     <xsd:import namespace="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
@@ -8642,15 +10480,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
@@ -8669,6 +10498,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5DF0EC-50CC-41C3-B7FF-8028A891B995}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8685,12 +10522,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Weapon generation | Change | diceNumber and damge based on the rarity, the gripType and weaponType
</commit_message>
<xml_diff>
--- a/Liste des évolutions.xlsx
+++ b/Liste des évolutions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u049298\Desktop\PYTHON_DJANGO\projetWebRPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B49D30-2CF4-4D57-B156-872DF15651AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB997E6-82B1-4AE3-9DAC-104ED479E9BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0\D"/>
+    <numFmt numFmtId="164" formatCode="0\D"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -625,9 +625,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -647,7 +644,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -7731,8 +7731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:BK37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -7750,11 +7750,12 @@
     <col min="22" max="22" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="29" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="40" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="40" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="7.5" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="6.1640625" bestFit="1" customWidth="1"/>
@@ -7767,75 +7768,75 @@
         <v>101</v>
       </c>
       <c r="E2" s="20"/>
-      <c r="I2" s="30">
+      <c r="I2" s="29">
         <v>1</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="29">
         <v>2</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="29">
         <v>3</v>
       </c>
-      <c r="L2" s="30">
+      <c r="L2" s="29">
         <v>4</v>
       </c>
-      <c r="M2" s="24"/>
-      <c r="P2" s="26">
+      <c r="M2" s="23"/>
+      <c r="P2" s="25">
         <v>4</v>
       </c>
-      <c r="Q2" s="26">
+      <c r="Q2" s="25">
         <v>6</v>
       </c>
-      <c r="R2" s="26">
+      <c r="R2" s="25">
         <v>8</v>
       </c>
-      <c r="S2" s="26">
+      <c r="S2" s="25">
         <v>10</v>
       </c>
-      <c r="T2" s="26">
+      <c r="T2" s="25">
         <v>12</v>
       </c>
-      <c r="U2" s="26">
+      <c r="U2" s="25">
         <v>20</v>
       </c>
-      <c r="V2" s="26">
+      <c r="V2" s="25">
         <v>100</v>
       </c>
-      <c r="W2" s="24"/>
-      <c r="Z2" s="26">
+      <c r="W2" s="23"/>
+      <c r="Z2" s="25">
         <v>1</v>
       </c>
-      <c r="AA2" s="26">
+      <c r="AA2" s="25">
         <v>2</v>
       </c>
-      <c r="AB2" s="26">
+      <c r="AB2" s="25">
         <v>3</v>
       </c>
-      <c r="AC2" s="26">
+      <c r="AC2" s="25">
         <v>4</v>
       </c>
-      <c r="AH2" s="26">
+      <c r="AH2" s="25">
         <v>4</v>
       </c>
-      <c r="AI2" s="26">
+      <c r="AI2" s="25">
         <v>6</v>
       </c>
-      <c r="AJ2" s="26">
+      <c r="AJ2" s="25">
         <v>8</v>
       </c>
-      <c r="AK2" s="26">
+      <c r="AK2" s="25">
         <v>10</v>
       </c>
-      <c r="AL2" s="26">
+      <c r="AL2" s="25">
         <v>12</v>
       </c>
-      <c r="AM2" s="26">
+      <c r="AM2" s="25">
         <v>20</v>
       </c>
-      <c r="AN2" s="26">
+      <c r="AN2" s="25">
         <v>100</v>
       </c>
-      <c r="AO2" s="24"/>
+      <c r="AO2" s="23"/>
     </row>
     <row r="3" spans="2:63" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -7847,111 +7848,111 @@
       <c r="E3" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I3" s="26">
+      <c r="I3" s="25">
         <v>80</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="25">
         <v>19</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="25">
         <v>1</v>
       </c>
-      <c r="L3" s="26">
+      <c r="L3" s="25">
         <v>0</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="26" t="s">
         <v>90</v>
       </c>
       <c r="N3">
         <f>($I$2*I3+$J$2*J3+$K$2*K3+$L$2*L3)/SUM(I3:L3)</f>
         <v>1.21</v>
       </c>
-      <c r="P3" s="26">
+      <c r="P3" s="25">
         <v>60</v>
       </c>
-      <c r="Q3" s="26">
+      <c r="Q3" s="25">
         <v>25</v>
       </c>
-      <c r="R3" s="26">
+      <c r="R3" s="25">
         <v>10</v>
       </c>
-      <c r="S3" s="26">
+      <c r="S3" s="25">
         <v>5</v>
       </c>
-      <c r="T3" s="26">
+      <c r="T3" s="25">
         <v>0</v>
       </c>
-      <c r="U3" s="26">
+      <c r="U3" s="25">
         <v>0</v>
       </c>
-      <c r="V3" s="26">
+      <c r="V3" s="25">
         <v>0</v>
       </c>
-      <c r="W3" s="27" t="s">
+      <c r="W3" s="26" t="s">
         <v>108</v>
       </c>
       <c r="X3">
         <f>(P3*$P$2+Q3*$Q$2+R3*$R$2+S3*$S$2+T3*$T$2+U3*$U$2+V3*$V$2)/SUM(P3:V3)</f>
         <v>5.2</v>
       </c>
-      <c r="Z3" s="29">
-        <f>I9/200+I3/200</f>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="AA3" s="29">
-        <f t="shared" ref="AA3:AC3" si="0">J9/200+J3/200</f>
-        <v>0.14500000000000002</v>
-      </c>
-      <c r="AB3" s="29">
+      <c r="Z3" s="28">
+        <f>(I$9+I3)/200</f>
+        <v>0.85</v>
+      </c>
+      <c r="AA3" s="28">
+        <f t="shared" ref="AA3:AC6" si="0">(J$9+J3)/200</f>
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AB3" s="28">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AC3" s="29">
+      <c r="AC3" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD3" s="27" t="s">
+      <c r="AD3" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="AE3" s="27" t="s">
+      <c r="AE3" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AF3">
         <f>($Z$2*Z3+$AA$2*AA3+$AB$2*AB3+$AC$2*AC3)/SUM(Z3:AC3)</f>
-        <v>1.155</v>
-      </c>
-      <c r="AH3" s="29">
-        <f>P3/200+P11/200</f>
+        <v>1.1549999999999998</v>
+      </c>
+      <c r="AH3" s="28">
+        <f>(P$3+P11)/200</f>
         <v>0.39500000000000002</v>
       </c>
-      <c r="AI3" s="29">
-        <f>Q3/200+Q11/200</f>
+      <c r="AI3" s="28">
+        <f>(Q3+Q$11)/200</f>
         <v>0.47499999999999998</v>
       </c>
-      <c r="AJ3" s="29">
-        <f>R3/200+R11/200</f>
+      <c r="AJ3" s="28">
+        <f t="shared" ref="AI3:AN3" si="1">(R3+R$11)/200</f>
         <v>0.1</v>
       </c>
-      <c r="AK3" s="29">
-        <f>S3/200+S11/200</f>
-        <v>3.0000000000000002E-2</v>
-      </c>
-      <c r="AL3" s="29">
-        <f>T3/200+T11/200</f>
+      <c r="AK3" s="28">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="AL3" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AM3" s="29">
-        <f>U3/200+U11/200</f>
+      <c r="AM3" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AN3" s="29">
-        <f>V3/200+V11/200</f>
+      <c r="AN3" s="28">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AO3" s="27" t="s">
+      <c r="AO3" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AP3" s="27" t="s">
+      <c r="AP3" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AQ3">
@@ -7975,115 +7976,115 @@
       <c r="E4" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="26">
+      <c r="I4" s="25">
         <v>70</v>
       </c>
-      <c r="J4" s="26">
+      <c r="J4" s="25">
         <v>28</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="25">
         <v>2</v>
       </c>
-      <c r="L4" s="26">
+      <c r="L4" s="25">
         <v>0</v>
       </c>
-      <c r="M4" s="27" t="s">
+      <c r="M4" s="26" t="s">
         <v>91</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N6" si="1">($I$2*I4+$J$2*J4+$K$2*K4+$L$2*L4)/SUM(I4:L4)</f>
+        <f t="shared" ref="N4:N6" si="2">($I$2*I4+$J$2*J4+$K$2*K4+$L$2*L4)/SUM(I4:L4)</f>
         <v>1.32</v>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="25">
         <v>0</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="25">
         <v>20</v>
       </c>
-      <c r="R4" s="26">
+      <c r="R4" s="25">
         <v>50</v>
       </c>
-      <c r="S4" s="26">
+      <c r="S4" s="25">
         <v>20</v>
       </c>
-      <c r="T4" s="26">
+      <c r="T4" s="25">
         <v>9</v>
       </c>
-      <c r="U4" s="26">
+      <c r="U4" s="25">
         <v>1</v>
       </c>
-      <c r="V4" s="26">
+      <c r="V4" s="25">
         <v>0</v>
       </c>
-      <c r="W4" s="27" t="s">
+      <c r="W4" s="26" t="s">
         <v>141</v>
       </c>
       <c r="X4">
-        <f t="shared" ref="X4:X8" si="2">(P4*$P$2+Q4*$Q$2+R4*$R$2+S4*$S$2+T4*$T$2+U4*$U$2+V4*$V$2)/SUM(P4:V4)</f>
+        <f t="shared" ref="X4:X8" si="3">(P4*$P$2+Q4*$Q$2+R4*$R$2+S4*$S$2+T4*$T$2+U4*$U$2+V4*$V$2)/SUM(P4:V4)</f>
         <v>8.48</v>
       </c>
-      <c r="Z4" s="29">
-        <f>I9/200+I4/200</f>
+      <c r="Z4" s="28">
+        <f t="shared" ref="Z4:Z6" si="4">(I$9+I4)/200</f>
         <v>0.8</v>
       </c>
-      <c r="AA4" s="29">
-        <f t="shared" ref="AA4:AC4" si="3">J9/200+J4/200</f>
+      <c r="AA4" s="28">
+        <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-      <c r="AB4" s="29">
-        <f t="shared" si="3"/>
+      <c r="AB4" s="28">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="AC4" s="29">
-        <f t="shared" si="3"/>
+      <c r="AC4" s="28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AD4" s="27" t="s">
+      <c r="AD4" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="AE4" s="27" t="s">
+      <c r="AE4" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AF4">
-        <f t="shared" ref="AF4:AF14" si="4">($Z$2*Z4+$AA$2*AA4+$AB$2*AB4+$AC$2*AC4)/SUM(Z4:AC4)</f>
+        <f t="shared" ref="AF4:AF14" si="5">($Z$2*Z4+$AA$2*AA4+$AB$2*AB4+$AC$2*AC4)/SUM(Z4:AC4)</f>
         <v>1.2100000000000002</v>
       </c>
-      <c r="AH4" s="29">
-        <f>P3/200+P12/200</f>
+      <c r="AH4" s="28">
+        <f t="shared" ref="AH4:AH6" si="6">(P$3+P12)/200</f>
         <v>0.3</v>
       </c>
-      <c r="AI4" s="29">
-        <f>Q3/200+Q12/200</f>
+      <c r="AI4" s="28">
+        <f t="shared" ref="AI4:AI5" si="7">(Q$3+Q12)/200</f>
         <v>0.3</v>
       </c>
-      <c r="AJ4" s="29">
-        <f>R3/200+R12/200</f>
+      <c r="AJ4" s="28">
+        <f t="shared" ref="AJ4:AJ5" si="8">(R$3+R12)/200</f>
         <v>0.32</v>
       </c>
-      <c r="AK4" s="29">
-        <f>S3/200+S12/200</f>
-        <v>7.5000000000000011E-2</v>
-      </c>
-      <c r="AL4" s="29">
-        <f>T3/200+T12/200</f>
+      <c r="AK4" s="28">
+        <f t="shared" ref="AK4:AK5" si="9">(S$3+S12)/200</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AL4" s="28">
+        <f t="shared" ref="AL4:AL5" si="10">(T$3+T12)/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AM4" s="29">
-        <f>U3/200+U12/200</f>
+      <c r="AM4" s="28">
+        <f t="shared" ref="AM4:AM5" si="11">(U$3+U12)/200</f>
         <v>0</v>
       </c>
-      <c r="AN4" s="29">
-        <f>V3/200+V12/200</f>
+      <c r="AN4" s="28">
+        <f t="shared" ref="AN4:AN5" si="12">(V$3+V12)/200</f>
         <v>0</v>
       </c>
-      <c r="AO4" s="27" t="s">
+      <c r="AO4" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AP4" s="27" t="s">
+      <c r="AP4" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ4">
-        <f t="shared" ref="AQ4:AQ26" si="5">($AH$2*AH4+$AI$2*AI4+$AJ$2*AJ4+$AK$2*AK4+$AL$2*AL4+$AM$2*AM4+$AN$2*AN4)/SUM(AH4:AN4)</f>
+        <f t="shared" ref="AQ4:AQ26" si="13">($AH$2*AH4+$AI$2*AI4+$AJ$2*AJ4+$AK$2*AK4+$AL$2*AL4+$AM$2*AM4+$AN$2*AN4)/SUM(AH4:AN4)</f>
         <v>6.370000000000001</v>
       </c>
       <c r="BI4" t="s">
@@ -8103,115 +8104,115 @@
       <c r="E5" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="25">
         <v>50</v>
       </c>
-      <c r="J5" s="26">
+      <c r="J5" s="25">
         <v>39</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="25">
         <v>10</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="25">
         <v>1</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="26" t="s">
         <v>92</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.62</v>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="25">
         <v>5</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="25">
         <v>25</v>
       </c>
-      <c r="R5" s="26">
+      <c r="R5" s="25">
         <v>35</v>
       </c>
-      <c r="S5" s="26">
+      <c r="S5" s="25">
         <v>25</v>
       </c>
-      <c r="T5" s="26">
+      <c r="T5" s="25">
         <v>9</v>
       </c>
-      <c r="U5" s="26">
+      <c r="U5" s="25">
         <v>1</v>
       </c>
-      <c r="V5" s="26">
+      <c r="V5" s="25">
         <v>0</v>
       </c>
-      <c r="W5" s="27" t="s">
+      <c r="W5" s="26" t="s">
         <v>103</v>
       </c>
       <c r="X5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.2799999999999994</v>
       </c>
-      <c r="Z5" s="29">
-        <f>I9/200+I5/200</f>
+      <c r="Z5" s="28">
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
-      <c r="AA5" s="29">
-        <f t="shared" ref="AA5:AC5" si="6">J9/200+J5/200</f>
+      <c r="AA5" s="28">
+        <f t="shared" si="0"/>
         <v>0.245</v>
       </c>
-      <c r="AB5" s="29">
-        <f t="shared" si="6"/>
+      <c r="AB5" s="28">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AC5" s="29">
-        <f t="shared" si="6"/>
+      <c r="AC5" s="28">
+        <f t="shared" si="0"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AD5" s="27" t="s">
+      <c r="AD5" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="AE5" s="27" t="s">
+      <c r="AE5" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3599999999999999</v>
       </c>
-      <c r="AH5" s="29">
-        <f>P3/200+P13/200</f>
+      <c r="AH5" s="28">
+        <f>(P$3+P13)/200</f>
         <v>0.3</v>
       </c>
-      <c r="AI5" s="29">
-        <f>Q3/200+Q13/200</f>
+      <c r="AI5" s="28">
+        <f>(Q$3+Q13)/200</f>
         <v>0.125</v>
       </c>
-      <c r="AJ5" s="29">
-        <f>R3/200+R13/200</f>
+      <c r="AJ5" s="28">
+        <f t="shared" si="8"/>
         <v>0.3</v>
       </c>
-      <c r="AK5" s="29">
-        <f>S3/200+S13/200</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="AL5" s="29">
-        <f>T3/200+T13/200</f>
+      <c r="AK5" s="28">
+        <f t="shared" si="9"/>
+        <v>0.2</v>
+      </c>
+      <c r="AL5" s="28">
+        <f t="shared" si="10"/>
         <v>0.05</v>
       </c>
-      <c r="AM5" s="29">
-        <f>U3/200+U13/200</f>
+      <c r="AM5" s="28">
+        <f t="shared" si="11"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AN5" s="29">
-        <f>V3/200+V13/200</f>
+      <c r="AN5" s="28">
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="AO5" s="27" t="s">
+      <c r="AO5" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AP5" s="27" t="s">
+      <c r="AP5" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>7.4499999999999993</v>
       </c>
       <c r="BI5" t="s">
@@ -8231,115 +8232,115 @@
       <c r="E6" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="26">
+      <c r="I6" s="25">
         <v>0</v>
       </c>
-      <c r="J6" s="26">
+      <c r="J6" s="25">
         <v>60</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="25">
         <v>30</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="25">
         <v>10</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="26" t="s">
         <v>99</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
-      <c r="P6" s="26">
+      <c r="P6" s="25">
         <v>0</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="Q6" s="25">
         <v>0</v>
       </c>
-      <c r="R6" s="26">
+      <c r="R6" s="25">
         <v>20</v>
       </c>
-      <c r="S6" s="26">
+      <c r="S6" s="25">
         <v>60</v>
       </c>
-      <c r="T6" s="26">
+      <c r="T6" s="25">
         <v>18</v>
       </c>
-      <c r="U6" s="26">
+      <c r="U6" s="25">
         <v>2</v>
       </c>
-      <c r="V6" s="26">
+      <c r="V6" s="25">
         <v>0</v>
       </c>
-      <c r="W6" s="27" t="s">
+      <c r="W6" s="26" t="s">
         <v>124</v>
       </c>
       <c r="X6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.16</v>
       </c>
-      <c r="Z6" s="29">
-        <f>I9/200+I6/200</f>
+      <c r="Z6" s="28">
+        <f t="shared" si="4"/>
         <v>0.45</v>
       </c>
-      <c r="AA6" s="29">
-        <f t="shared" ref="AA6:AC6" si="7">J9/200+J6/200</f>
+      <c r="AA6" s="28">
+        <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="AB6" s="29">
-        <f t="shared" si="7"/>
+      <c r="AB6" s="28">
+        <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="AC6" s="29">
-        <f t="shared" si="7"/>
+      <c r="AC6" s="28">
+        <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
-      <c r="AD6" s="27" t="s">
+      <c r="AD6" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="AE6" s="27" t="s">
+      <c r="AE6" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AF6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="AH6" s="29">
-        <f>P3/200+P14/200</f>
+      <c r="AH6" s="28">
+        <f>(P$3+P14)/200</f>
         <v>0.3</v>
       </c>
-      <c r="AI6" s="29">
-        <f>Q3/200+Q14/200</f>
+      <c r="AI6" s="28">
+        <f>(Q$3+Q14)/200</f>
         <v>0.125</v>
       </c>
-      <c r="AJ6" s="29">
-        <f>R3/200+R14/200</f>
+      <c r="AJ6" s="28">
+        <f>(R$3+R14)/200</f>
         <v>0.05</v>
       </c>
-      <c r="AK6" s="29">
-        <f>S3/200+S14/200</f>
+      <c r="AK6" s="28">
+        <f>(S$3+S14)/200</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AL6" s="29">
-        <f>T3/200+T14/200</f>
+      <c r="AL6" s="28">
+        <f>(T$3+T14)/200</f>
         <v>0.15</v>
       </c>
-      <c r="AM6" s="29">
-        <f>U3/200+U14/200</f>
+      <c r="AM6" s="28">
+        <f>(U$3+U14)/200</f>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AN6" s="29">
-        <f>V3/200+V14/200</f>
+      <c r="AN6" s="28">
+        <f>(V$3+V14)/200</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AO6" s="27" t="s">
+      <c r="AO6" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AP6" s="27" t="s">
+      <c r="AP6" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AQ6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>9.2999999999999989</v>
       </c>
       <c r="BI6" t="s">
@@ -8357,97 +8358,97 @@
         <v>6</v>
       </c>
       <c r="E7" s="20"/>
-      <c r="P7" s="26">
+      <c r="P7" s="25">
         <v>15</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="Q7" s="25">
         <v>30</v>
       </c>
-      <c r="R7" s="26">
+      <c r="R7" s="25">
         <v>35</v>
       </c>
-      <c r="S7" s="26">
+      <c r="S7" s="25">
         <v>10</v>
       </c>
-      <c r="T7" s="26">
+      <c r="T7" s="25">
         <v>8</v>
       </c>
-      <c r="U7" s="26">
+      <c r="U7" s="25">
         <v>2</v>
       </c>
-      <c r="V7" s="26">
+      <c r="V7" s="25">
         <v>0</v>
       </c>
-      <c r="W7" s="28" t="s">
+      <c r="W7" s="27" t="s">
         <v>117</v>
       </c>
       <c r="X7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.56</v>
       </c>
-      <c r="Z7" s="29">
-        <f>I10/200+I3/200</f>
-        <v>0.44</v>
-      </c>
-      <c r="AA7" s="29">
-        <f t="shared" ref="AA7:AC7" si="8">J10/200+J3/200</f>
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="AB7" s="29">
-        <f t="shared" si="8"/>
+      <c r="Z7" s="28">
+        <f>(I$10+I3)/200</f>
+        <v>0.5</v>
+      </c>
+      <c r="AA7" s="28">
+        <f t="shared" ref="AA7:AC10" si="14">(J$10+J3)/200</f>
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="AB7" s="28">
+        <f t="shared" si="14"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AC7" s="29">
-        <f t="shared" si="8"/>
+      <c r="AC7" s="28">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="27" t="s">
+      <c r="AD7" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AE7" s="27" t="s">
+      <c r="AE7" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="4"/>
-        <v>1.575</v>
-      </c>
-      <c r="AH7" s="29">
-        <f>P$4/200+P11/200</f>
+        <f t="shared" si="5"/>
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="AH7" s="28">
+        <f>(P$4+P11)/200</f>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AI7" s="29">
-        <f>Q$4/200+Q11/200</f>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="AJ7" s="29">
-        <f>R$4/200+R11/200</f>
+      <c r="AI7" s="28">
+        <f t="shared" ref="AI7:AN7" si="15">(Q$4+Q11)/200</f>
+        <v>0.45</v>
+      </c>
+      <c r="AJ7" s="28">
+        <f t="shared" si="15"/>
         <v>0.3</v>
       </c>
-      <c r="AK7" s="29">
-        <f>S$4/200+S11/200</f>
-        <v>0.10500000000000001</v>
-      </c>
-      <c r="AL7" s="29">
-        <f>T$4/200+T11/200</f>
+      <c r="AK7" s="28">
+        <f t="shared" si="15"/>
+        <v>0.105</v>
+      </c>
+      <c r="AL7" s="28">
+        <f t="shared" si="15"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="AM7" s="29">
-        <f>U$4/200+U11/200</f>
+      <c r="AM7" s="28">
+        <f t="shared" si="15"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AN7" s="29">
-        <f>V$4/200+V11/200</f>
+      <c r="AN7" s="28">
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AO7" s="27" t="s">
+      <c r="AO7" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="AP7" s="27" t="s">
+      <c r="AP7" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="5"/>
-        <v>7.169999999999999</v>
+        <f t="shared" si="13"/>
+        <v>7.17</v>
       </c>
       <c r="BI7" t="s">
         <v>106</v>
@@ -8458,109 +8459,109 @@
     </row>
     <row r="8" spans="2:63" x14ac:dyDescent="0.2">
       <c r="E8" s="20"/>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>1</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="29">
         <v>2</v>
       </c>
-      <c r="K8" s="30">
+      <c r="K8" s="29">
         <v>3</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="29">
         <v>4</v>
       </c>
-      <c r="M8" s="24"/>
-      <c r="P8" s="26">
+      <c r="M8" s="23"/>
+      <c r="P8" s="25">
         <v>20</v>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="25">
         <v>35</v>
       </c>
-      <c r="R8" s="26">
+      <c r="R8" s="25">
         <v>25</v>
       </c>
-      <c r="S8" s="26">
+      <c r="S8" s="25">
         <v>10</v>
       </c>
-      <c r="T8" s="26">
+      <c r="T8" s="25">
         <v>7</v>
       </c>
-      <c r="U8" s="26">
+      <c r="U8" s="25">
         <v>3</v>
       </c>
-      <c r="V8" s="26">
+      <c r="V8" s="25">
         <v>0</v>
       </c>
-      <c r="W8" s="28" t="s">
+      <c r="W8" s="27" t="s">
         <v>106</v>
       </c>
       <c r="X8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.34</v>
       </c>
-      <c r="Z8" s="29">
-        <f>I10/200+I4/200</f>
-        <v>0.38999999999999996</v>
-      </c>
-      <c r="AA8" s="29">
-        <f t="shared" ref="AA8:AC8" si="9">J10/200+J4/200</f>
-        <v>0.59000000000000008</v>
-      </c>
-      <c r="AB8" s="29">
-        <f t="shared" si="9"/>
+      <c r="Z8" s="28">
+        <f t="shared" ref="Z8:Z10" si="16">(I$10+I4)/200</f>
+        <v>0.45</v>
+      </c>
+      <c r="AA8" s="28">
+        <f t="shared" si="14"/>
+        <v>0.53</v>
+      </c>
+      <c r="AB8" s="28">
+        <f t="shared" si="14"/>
         <v>0.02</v>
       </c>
-      <c r="AC8" s="29">
-        <f t="shared" si="9"/>
+      <c r="AC8" s="28">
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="AD8" s="27" t="s">
+      <c r="AD8" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AE8" s="27" t="s">
+      <c r="AE8" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AF8">
-        <f t="shared" si="4"/>
-        <v>1.6300000000000001</v>
-      </c>
-      <c r="AH8" s="29">
-        <f>P$4/200+P12/200</f>
+        <f t="shared" si="5"/>
+        <v>1.57</v>
+      </c>
+      <c r="AH8" s="28">
+        <f>(P$4+P12)/200</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="29">
-        <f>Q$4/200+Q12/200</f>
+      <c r="AI8" s="28">
+        <f t="shared" ref="AI8:AN10" si="17">(Q$4+Q12)/200</f>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AJ8" s="29">
-        <f>R$4/200+R12/200</f>
+      <c r="AJ8" s="28">
+        <f t="shared" si="17"/>
         <v>0.52</v>
       </c>
-      <c r="AK8" s="29">
-        <f>S$4/200+S12/200</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="AL8" s="29">
-        <f>T$4/200+T12/200</f>
-        <v>4.9999999999999996E-2</v>
-      </c>
-      <c r="AM8" s="29">
-        <f>U$4/200+U12/200</f>
+      <c r="AK8" s="28">
+        <f t="shared" si="17"/>
+        <v>0.15</v>
+      </c>
+      <c r="AL8" s="28">
+        <f t="shared" si="17"/>
+        <v>0.05</v>
+      </c>
+      <c r="AM8" s="28">
+        <f t="shared" si="17"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AN8" s="29">
-        <f>V$4/200+V12/200</f>
+      <c r="AN8" s="28">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AO8" s="27" t="s">
+      <c r="AO8" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="AP8" s="27" t="s">
+      <c r="AP8" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.01</v>
       </c>
       <c r="BI8" t="s">
@@ -8575,87 +8576,87 @@
         <v>94</v>
       </c>
       <c r="E9" s="20"/>
-      <c r="I9" s="26">
+      <c r="I9" s="25">
         <v>90</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="25">
         <v>10</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="25">
         <v>0</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="25">
         <v>0</v>
       </c>
-      <c r="M9" s="27" t="s">
+      <c r="M9" s="26" t="s">
         <v>138</v>
       </c>
       <c r="N9">
         <f>($I$2*I9+$J$2*J9+$K$2*K9+$L$2*L9)/SUM(I9:L9)</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="Z9" s="29">
-        <f>I10/200+I5/200</f>
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="AA9" s="29">
-        <f t="shared" ref="AA9:AC9" si="10">J10/200+J5/200</f>
-        <v>0.64500000000000002</v>
-      </c>
-      <c r="AB9" s="29">
-        <f t="shared" si="10"/>
-        <v>6.0000000000000005E-2</v>
-      </c>
-      <c r="AC9" s="29">
-        <f t="shared" si="10"/>
+      <c r="Z9" s="28">
+        <f t="shared" si="16"/>
+        <v>0.35</v>
+      </c>
+      <c r="AA9" s="28">
+        <f t="shared" si="14"/>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="AB9" s="28">
+        <f t="shared" si="14"/>
+        <v>0.06</v>
+      </c>
+      <c r="AC9" s="28">
+        <f t="shared" si="14"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AD9" s="27" t="s">
+      <c r="AD9" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="AE9" s="27" t="s">
+      <c r="AE9" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="4"/>
-        <v>1.78</v>
-      </c>
-      <c r="AH9" s="29">
-        <f>P$4/200+P13/200</f>
+        <f t="shared" si="5"/>
+        <v>1.7200000000000002</v>
+      </c>
+      <c r="AH9" s="28">
+        <f t="shared" ref="AH8:AH10" si="18">(P$4+P13)/200</f>
         <v>0</v>
       </c>
-      <c r="AI9" s="29">
-        <f>Q$4/200+Q13/200</f>
+      <c r="AI9" s="28">
+        <f t="shared" si="17"/>
         <v>0.1</v>
       </c>
-      <c r="AJ9" s="29">
-        <f>R$4/200+R13/200</f>
+      <c r="AJ9" s="28">
+        <f t="shared" si="17"/>
         <v>0.5</v>
       </c>
-      <c r="AK9" s="29">
-        <f>S$4/200+S13/200</f>
+      <c r="AK9" s="28">
+        <f t="shared" si="17"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="AL9" s="29">
-        <f>T$4/200+T13/200</f>
+      <c r="AL9" s="28">
+        <f t="shared" si="17"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AM9" s="29">
-        <f>U$4/200+U13/200</f>
-        <v>3.0000000000000002E-2</v>
-      </c>
-      <c r="AN9" s="29">
-        <f>V$4/200+V13/200</f>
+      <c r="AM9" s="28">
+        <f t="shared" si="17"/>
+        <v>0.03</v>
+      </c>
+      <c r="AN9" s="28">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AO9" s="27" t="s">
+      <c r="AO9" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="AP9" s="27" t="s">
+      <c r="AP9" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AQ9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>9.09</v>
       </c>
       <c r="BI9" t="s">
@@ -8670,108 +8671,108 @@
         <v>96</v>
       </c>
       <c r="E10" s="20"/>
-      <c r="I10" s="26">
+      <c r="I10" s="25">
+        <v>20</v>
+      </c>
+      <c r="J10" s="25">
+        <v>78</v>
+      </c>
+      <c r="K10" s="25">
+        <v>2</v>
+      </c>
+      <c r="L10" s="25">
+        <v>0</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10:N11" si="19">($I$2*I10+$J$2*J10+$K$2*K10+$L$2*L10)/SUM(I10:L10)</f>
+        <v>1.82</v>
+      </c>
+      <c r="P10" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="25">
+        <v>6</v>
+      </c>
+      <c r="R10" s="25">
         <v>8</v>
       </c>
-      <c r="J10" s="26">
-        <v>90</v>
-      </c>
-      <c r="K10" s="26">
-        <v>2</v>
-      </c>
-      <c r="L10" s="26">
+      <c r="S10" s="25">
+        <v>10</v>
+      </c>
+      <c r="T10" s="25">
+        <v>12</v>
+      </c>
+      <c r="U10" s="25">
+        <v>20</v>
+      </c>
+      <c r="V10" s="25">
+        <v>100</v>
+      </c>
+      <c r="Z10" s="28">
+        <f t="shared" si="16"/>
+        <v>0.1</v>
+      </c>
+      <c r="AA10" s="28">
+        <f>(J$10+J6)/200 +Z10</f>
+        <v>0.78999999999999992</v>
+      </c>
+      <c r="AB10" s="28">
+        <f t="shared" ref="AB10:AC10" si="20">(K$10+K6)/200 +AA10</f>
+        <v>0.95</v>
+      </c>
+      <c r="AC10" s="28">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AD10" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE10" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="5"/>
+        <v>3.0035211267605635</v>
+      </c>
+      <c r="AH10" s="28">
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="M10" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="N10">
-        <f t="shared" ref="N10:N12" si="11">($I$2*I10+$J$2*J10+$K$2*K10+$L$2*L10)/SUM(I10:L10)</f>
-        <v>1.94</v>
-      </c>
-      <c r="P10" s="26">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="26">
-        <v>6</v>
-      </c>
-      <c r="R10" s="26">
-        <v>8</v>
-      </c>
-      <c r="S10" s="26">
-        <v>10</v>
-      </c>
-      <c r="T10" s="26">
-        <v>12</v>
-      </c>
-      <c r="U10" s="26">
-        <v>20</v>
-      </c>
-      <c r="V10" s="26">
-        <v>100</v>
-      </c>
-      <c r="Z10" s="29">
-        <f>I10/200+I6/200</f>
-        <v>0.04</v>
-      </c>
-      <c r="AA10" s="29">
-        <f t="shared" ref="AA10:AC10" si="12">J10/200+J6/200</f>
-        <v>0.75</v>
-      </c>
-      <c r="AB10" s="29">
-        <f t="shared" si="12"/>
-        <v>0.16</v>
-      </c>
-      <c r="AC10" s="29">
-        <f t="shared" si="12"/>
-        <v>0.05</v>
-      </c>
-      <c r="AD10" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="AE10" s="27" t="s">
+      <c r="AI10" s="28">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="AJ10" s="28">
+        <f t="shared" si="17"/>
+        <v>0.25</v>
+      </c>
+      <c r="AK10" s="28">
+        <f t="shared" si="17"/>
+        <v>0.35</v>
+      </c>
+      <c r="AL10" s="28">
+        <f t="shared" si="17"/>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AM10" s="28">
+        <f t="shared" si="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="AN10" s="28">
+        <f t="shared" si="17"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AO10" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="AP10" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="AF10">
-        <f t="shared" si="4"/>
-        <v>2.2200000000000002</v>
-      </c>
-      <c r="AH10" s="29">
-        <f>P$4/200+P14/200</f>
-        <v>0</v>
-      </c>
-      <c r="AI10" s="29">
-        <f>Q$4/200+Q14/200</f>
-        <v>0.1</v>
-      </c>
-      <c r="AJ10" s="29">
-        <f>R$4/200+R14/200</f>
-        <v>0.25</v>
-      </c>
-      <c r="AK10" s="29">
-        <f>S$4/200+S14/200</f>
-        <v>0.35</v>
-      </c>
-      <c r="AL10" s="29">
-        <f>T$4/200+T14/200</f>
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="AM10" s="29">
-        <f>U$4/200+U14/200</f>
-        <v>0.1</v>
-      </c>
-      <c r="AN10" s="29">
-        <f>V$4/200+V14/200</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AO10" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="AP10" s="27" t="s">
-        <v>99</v>
-      </c>
       <c r="AQ10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>10.94</v>
       </c>
       <c r="BI10" t="s">
@@ -8786,116 +8787,116 @@
         <v>2</v>
       </c>
       <c r="E11" s="20"/>
-      <c r="I11" s="26">
+      <c r="I11" s="25">
         <v>60</v>
       </c>
-      <c r="J11" s="26">
+      <c r="J11" s="25">
         <v>35</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="25">
         <v>5</v>
       </c>
-      <c r="L11" s="26">
+      <c r="L11" s="25">
         <v>0</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="M11" s="26" t="s">
         <v>140</v>
       </c>
       <c r="N11">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>1.45</v>
       </c>
-      <c r="P11" s="26">
+      <c r="P11" s="25">
         <v>19</v>
       </c>
-      <c r="Q11" s="26">
+      <c r="Q11" s="25">
         <v>70</v>
       </c>
-      <c r="R11" s="26">
+      <c r="R11" s="25">
         <v>10</v>
       </c>
-      <c r="S11" s="26">
+      <c r="S11" s="25">
         <v>1</v>
       </c>
-      <c r="T11" s="26">
+      <c r="T11" s="25">
         <v>0</v>
       </c>
-      <c r="U11" s="26">
+      <c r="U11" s="25">
         <v>0</v>
       </c>
-      <c r="V11" s="26">
+      <c r="V11" s="25">
         <v>0</v>
       </c>
-      <c r="W11" s="27" t="s">
+      <c r="W11" s="26" t="s">
         <v>90</v>
       </c>
       <c r="X11">
         <f>(P11*$P$2+Q11*$Q$2+R11*$R$2+S11*$S$2+T11*$T$2+U11*$U$2+V11*$V$2)/SUM(P11:V11)</f>
         <v>5.86</v>
       </c>
-      <c r="Z11" s="29">
-        <f>I11/200+I3/200</f>
+      <c r="Z11" s="28">
+        <f>(I$11+I3)/200</f>
         <v>0.7</v>
       </c>
-      <c r="AA11" s="29">
-        <f t="shared" ref="AA11:AC11" si="13">J11/200+J3/200</f>
+      <c r="AA11" s="28">
+        <f t="shared" ref="AA11:AC14" si="21">(J$11+J3)/200</f>
         <v>0.27</v>
       </c>
-      <c r="AB11" s="29">
+      <c r="AB11" s="28">
+        <f t="shared" si="21"/>
+        <v>0.03</v>
+      </c>
+      <c r="AC11" s="28">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AF11">
+        <f t="shared" si="5"/>
+        <v>1.33</v>
+      </c>
+      <c r="AH11" s="28">
+        <f>(P$5+P11)/200</f>
+        <v>0.12</v>
+      </c>
+      <c r="AI11" s="28">
+        <f t="shared" ref="AI11:AN14" si="22">(Q$5+Q11)/200</f>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="AJ11" s="28">
+        <f t="shared" si="22"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AK11" s="28">
+        <f t="shared" si="22"/>
+        <v>0.13</v>
+      </c>
+      <c r="AL11" s="28">
+        <f t="shared" si="22"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AM11" s="28">
+        <f t="shared" si="22"/>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN11" s="28">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AO11" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="AP11" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ11">
         <f t="shared" si="13"/>
-        <v>3.0000000000000002E-2</v>
-      </c>
-      <c r="AC11" s="29">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="AD11" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE11" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF11">
-        <f t="shared" si="4"/>
-        <v>1.33</v>
-      </c>
-      <c r="AH11" s="29">
-        <f>P$5/200+P11/200</f>
-        <v>0.12</v>
-      </c>
-      <c r="AI11" s="29">
-        <f>Q$5/200+Q11/200</f>
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="AJ11" s="29">
-        <f>R$5/200+R11/200</f>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="AK11" s="29">
-        <f>S$5/200+S11/200</f>
-        <v>0.13</v>
-      </c>
-      <c r="AL11" s="29">
-        <f>T$5/200+T11/200</f>
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="AM11" s="29">
-        <f>U$5/200+U11/200</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="AN11" s="29">
-        <f>V$5/200+V11/200</f>
-        <v>0</v>
-      </c>
-      <c r="AO11" s="27" t="s">
-        <v>103</v>
-      </c>
-      <c r="AP11" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="AQ11">
-        <f t="shared" si="5"/>
-        <v>7.0699999999999985</v>
+        <v>7.0699999999999994</v>
       </c>
       <c r="BI11" t="s">
         <v>111</v>
@@ -8908,102 +8909,102 @@
       <c r="C12">
         <v>4</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="25"/>
-      <c r="P12" s="26">
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="24"/>
+      <c r="P12" s="25">
         <v>0</v>
       </c>
-      <c r="Q12" s="26">
+      <c r="Q12" s="25">
         <v>35</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="25">
         <v>54</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="25">
         <v>10</v>
       </c>
-      <c r="T12" s="26">
+      <c r="T12" s="25">
         <v>1</v>
       </c>
-      <c r="U12" s="26">
+      <c r="U12" s="25">
         <v>0</v>
       </c>
-      <c r="V12" s="26">
+      <c r="V12" s="25">
         <v>0</v>
       </c>
-      <c r="W12" s="27" t="s">
+      <c r="W12" s="26" t="s">
         <v>91</v>
       </c>
       <c r="X12">
-        <f t="shared" ref="X12:X14" si="14">(P12*$P$2+Q12*$Q$2+R12*$R$2+S12*$S$2+T12*$T$2+U12*$U$2+V12*$V$2)/SUM(P12:V12)</f>
+        <f t="shared" ref="X12:X14" si="23">(P12*$P$2+Q12*$Q$2+R12*$R$2+S12*$S$2+T12*$T$2+U12*$U$2+V12*$V$2)/SUM(P12:V12)</f>
         <v>7.54</v>
       </c>
-      <c r="Z12" s="29">
-        <f>I11/200+I4/200</f>
-        <v>0.64999999999999991</v>
-      </c>
-      <c r="AA12" s="29">
-        <f t="shared" ref="AA12:AC12" si="15">J11/200+J4/200</f>
+      <c r="Z12" s="28">
+        <f t="shared" ref="Z12:Z14" si="24">(I$11+I4)/200</f>
+        <v>0.65</v>
+      </c>
+      <c r="AA12" s="28">
+        <f t="shared" si="21"/>
         <v>0.315</v>
       </c>
-      <c r="AB12" s="29">
-        <f t="shared" si="15"/>
+      <c r="AB12" s="28">
+        <f t="shared" si="21"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AC12" s="29">
-        <f t="shared" si="15"/>
+      <c r="AC12" s="28">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AD12" s="27" t="s">
+      <c r="AD12" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="AE12" s="27" t="s">
+      <c r="AE12" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AF12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.385</v>
       </c>
-      <c r="AH12" s="29">
-        <f>P$5/200+P12/200</f>
+      <c r="AH12" s="28">
+        <f t="shared" ref="AH12:AH14" si="25">(P$5+P12)/200</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AI12" s="29">
-        <f>Q$5/200+Q12/200</f>
+      <c r="AI12" s="28">
+        <f t="shared" si="22"/>
         <v>0.3</v>
       </c>
-      <c r="AJ12" s="29">
-        <f>R$5/200+R12/200</f>
+      <c r="AJ12" s="28">
+        <f t="shared" si="22"/>
         <v>0.44500000000000001</v>
       </c>
-      <c r="AK12" s="29">
-        <f>S$5/200+S12/200</f>
+      <c r="AK12" s="28">
+        <f t="shared" si="22"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AL12" s="29">
-        <f>T$5/200+T12/200</f>
-        <v>4.9999999999999996E-2</v>
-      </c>
-      <c r="AM12" s="29">
-        <f>U$5/200+U12/200</f>
+      <c r="AL12" s="28">
+        <f t="shared" si="22"/>
+        <v>0.05</v>
+      </c>
+      <c r="AM12" s="28">
+        <f t="shared" si="22"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AN12" s="29">
-        <f>V$5/200+V12/200</f>
+      <c r="AN12" s="28">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AO12" s="27" t="s">
+      <c r="AO12" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="AP12" s="27" t="s">
+      <c r="AP12" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ12">
-        <f t="shared" si="5"/>
-        <v>7.9099999999999993</v>
+        <f t="shared" si="13"/>
+        <v>7.91</v>
       </c>
       <c r="BI12" t="s">
         <v>112</v>
@@ -9016,96 +9017,96 @@
       <c r="C13">
         <v>6</v>
       </c>
-      <c r="P13" s="26">
+      <c r="P13" s="25">
         <v>0</v>
       </c>
-      <c r="Q13" s="26">
+      <c r="Q13" s="25">
         <v>0</v>
       </c>
-      <c r="R13" s="26">
+      <c r="R13" s="25">
         <v>50</v>
       </c>
-      <c r="S13" s="26">
+      <c r="S13" s="25">
         <v>35</v>
       </c>
-      <c r="T13" s="26">
+      <c r="T13" s="25">
         <v>10</v>
       </c>
-      <c r="U13" s="26">
+      <c r="U13" s="25">
         <v>5</v>
       </c>
-      <c r="V13" s="26">
+      <c r="V13" s="25">
         <v>0</v>
       </c>
-      <c r="W13" s="27" t="s">
+      <c r="W13" s="26" t="s">
         <v>92</v>
       </c>
       <c r="X13">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="Z13" s="29">
-        <f>I11/200+I5/200</f>
+      <c r="Z13" s="28">
+        <f t="shared" si="24"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="AA13" s="29">
-        <f t="shared" ref="AA13:AC13" si="16">J11/200+J5/200</f>
+      <c r="AA13" s="28">
+        <f t="shared" si="21"/>
         <v>0.37</v>
       </c>
-      <c r="AB13" s="29">
-        <f t="shared" si="16"/>
-        <v>7.5000000000000011E-2</v>
-      </c>
-      <c r="AC13" s="29">
-        <f t="shared" si="16"/>
+      <c r="AB13" s="28">
+        <f t="shared" si="21"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC13" s="28">
+        <f t="shared" si="21"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AD13" s="27" t="s">
+      <c r="AD13" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="AE13" s="27" t="s">
+      <c r="AE13" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AF13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.5350000000000001</v>
       </c>
-      <c r="AH13" s="29">
-        <f>P$5/200+P13/200</f>
+      <c r="AH13" s="28">
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AI13" s="29">
-        <f>Q$5/200+Q13/200</f>
+      <c r="AI13" s="28">
+        <f t="shared" si="22"/>
         <v>0.125</v>
       </c>
-      <c r="AJ13" s="29">
-        <f>R$5/200+R13/200</f>
+      <c r="AJ13" s="28">
+        <f t="shared" si="22"/>
         <v>0.42499999999999999</v>
       </c>
-      <c r="AK13" s="29">
-        <f>S$5/200+S13/200</f>
+      <c r="AK13" s="28">
+        <f t="shared" si="22"/>
         <v>0.3</v>
       </c>
-      <c r="AL13" s="29">
-        <f>T$5/200+T13/200</f>
+      <c r="AL13" s="28">
+        <f t="shared" si="22"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AM13" s="29">
-        <f>U$5/200+U13/200</f>
-        <v>3.0000000000000002E-2</v>
-      </c>
-      <c r="AN13" s="29">
-        <f>V$5/200+V13/200</f>
+      <c r="AM13" s="28">
+        <f t="shared" si="22"/>
+        <v>0.03</v>
+      </c>
+      <c r="AN13" s="28">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="AO13" s="27" t="s">
+      <c r="AO13" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="AP13" s="27" t="s">
+      <c r="AP13" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AQ13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.99</v>
       </c>
       <c r="BI13" t="s">
@@ -9119,96 +9120,96 @@
       <c r="C14">
         <v>12</v>
       </c>
-      <c r="P14" s="26">
+      <c r="P14" s="25">
         <v>0</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="Q14" s="25">
         <v>0</v>
       </c>
-      <c r="R14" s="26">
+      <c r="R14" s="25">
         <v>0</v>
       </c>
-      <c r="S14" s="26">
+      <c r="S14" s="25">
         <v>50</v>
       </c>
-      <c r="T14" s="26">
+      <c r="T14" s="25">
         <v>30</v>
       </c>
-      <c r="U14" s="26">
+      <c r="U14" s="25">
         <v>19</v>
       </c>
-      <c r="V14" s="26">
+      <c r="V14" s="25">
         <v>1</v>
       </c>
-      <c r="W14" s="27" t="s">
+      <c r="W14" s="26" t="s">
         <v>99</v>
       </c>
       <c r="X14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>13.4</v>
       </c>
-      <c r="Z14" s="29">
-        <f>I11/200+I6/200</f>
+      <c r="Z14" s="28">
+        <f t="shared" si="24"/>
         <v>0.3</v>
       </c>
-      <c r="AA14" s="29">
-        <f t="shared" ref="AA14:AC14" si="17">J11/200+J6/200</f>
+      <c r="AA14" s="28">
+        <f t="shared" si="21"/>
         <v>0.47499999999999998</v>
       </c>
-      <c r="AB14" s="29">
-        <f t="shared" si="17"/>
+      <c r="AB14" s="28">
+        <f t="shared" si="21"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AC14" s="29">
-        <f t="shared" si="17"/>
+      <c r="AC14" s="28">
+        <f t="shared" si="21"/>
         <v>0.05</v>
       </c>
-      <c r="AD14" s="27" t="s">
+      <c r="AD14" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="AE14" s="27" t="s">
+      <c r="AE14" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AF14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9749999999999999</v>
       </c>
-      <c r="AH14" s="29">
-        <f>P$5/200+P14/200</f>
+      <c r="AH14" s="28">
+        <f t="shared" si="25"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="AI14" s="29">
-        <f>Q$5/200+Q14/200</f>
+      <c r="AI14" s="28">
+        <f t="shared" si="22"/>
         <v>0.125</v>
       </c>
-      <c r="AJ14" s="29">
-        <f>R$5/200+R14/200</f>
+      <c r="AJ14" s="28">
+        <f t="shared" si="22"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AK14" s="29">
-        <f>S$5/200+S14/200</f>
+      <c r="AK14" s="28">
+        <f t="shared" si="22"/>
         <v>0.375</v>
       </c>
-      <c r="AL14" s="29">
-        <f>T$5/200+T14/200</f>
+      <c r="AL14" s="28">
+        <f t="shared" si="22"/>
         <v>0.19500000000000001</v>
       </c>
-      <c r="AM14" s="29">
-        <f>U$5/200+U14/200</f>
+      <c r="AM14" s="28">
+        <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
-      <c r="AN14" s="29">
-        <f>V$5/200+V14/200</f>
+      <c r="AN14" s="28">
+        <f t="shared" si="22"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AO14" s="27" t="s">
+      <c r="AO14" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="AP14" s="27" t="s">
+      <c r="AP14" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AQ14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>10.84</v>
       </c>
       <c r="BI14" t="s">
@@ -9216,42 +9217,42 @@
       </c>
     </row>
     <row r="15" spans="2:63" x14ac:dyDescent="0.2">
-      <c r="AH15" s="29">
-        <f>P$6/200+P11/200</f>
+      <c r="AH15" s="28">
+        <f>(P$6+P11)/200</f>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AI15" s="29">
-        <f>Q$6/200+Q11/200</f>
+      <c r="AI15" s="28">
+        <f t="shared" ref="AI15:AN18" si="26">(Q$6+Q11)/200</f>
         <v>0.35</v>
       </c>
-      <c r="AJ15" s="29">
-        <f>R$6/200+R11/200</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="AK15" s="29">
-        <f>S$6/200+S11/200</f>
+      <c r="AJ15" s="28">
+        <f t="shared" si="26"/>
+        <v>0.15</v>
+      </c>
+      <c r="AK15" s="28">
+        <f t="shared" si="26"/>
         <v>0.30499999999999999</v>
       </c>
-      <c r="AL15" s="29">
-        <f>T$6/200+T11/200</f>
+      <c r="AL15" s="28">
+        <f t="shared" si="26"/>
         <v>0.09</v>
       </c>
-      <c r="AM15" s="29">
-        <f>U$6/200+U11/200</f>
+      <c r="AM15" s="28">
+        <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AN15" s="29">
-        <f>V$6/200+V11/200</f>
+      <c r="AN15" s="28">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AO15" s="27" t="s">
+      <c r="AO15" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AP15" s="27" t="s">
+      <c r="AP15" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AQ15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.0100000000000016</v>
       </c>
       <c r="BI15" t="s">
@@ -9259,49 +9260,49 @@
       </c>
     </row>
     <row r="16" spans="2:63" x14ac:dyDescent="0.2">
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="19"/>
-      <c r="AH16" s="29">
-        <f>P$6/200+P12/200</f>
+      <c r="AH16" s="28">
+        <f t="shared" ref="AH16:AH18" si="27">(P$6+P12)/200</f>
         <v>0</v>
       </c>
-      <c r="AI16" s="29">
-        <f>Q$6/200+Q12/200</f>
+      <c r="AI16" s="28">
+        <f t="shared" si="26"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AJ16" s="29">
-        <f>R$6/200+R12/200</f>
+      <c r="AJ16" s="28">
+        <f t="shared" si="26"/>
         <v>0.37</v>
       </c>
-      <c r="AK16" s="29">
-        <f>S$6/200+S12/200</f>
+      <c r="AK16" s="28">
+        <f t="shared" si="26"/>
         <v>0.35</v>
       </c>
-      <c r="AL16" s="29">
-        <f>T$6/200+T12/200</f>
+      <c r="AL16" s="28">
+        <f t="shared" si="26"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="AM16" s="29">
-        <f>U$6/200+U12/200</f>
+      <c r="AM16" s="28">
+        <f t="shared" si="26"/>
         <v>0.01</v>
       </c>
-      <c r="AN16" s="29">
-        <f>V$6/200+V12/200</f>
+      <c r="AN16" s="28">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="27" t="s">
+      <c r="AO16" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AP16" s="27" t="s">
+      <c r="AP16" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.8500000000000014</v>
       </c>
       <c r="BI16" t="s">
@@ -9327,43 +9328,43 @@
       <c r="G17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="O17" s="25"/>
-      <c r="AH17" s="29">
-        <f>P$6/200+P13/200</f>
+      <c r="O17" s="24"/>
+      <c r="AH17" s="28">
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AI17" s="29">
-        <f>Q$6/200+Q13/200</f>
+      <c r="AI17" s="28">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AJ17" s="29">
-        <f>R$6/200+R13/200</f>
+      <c r="AJ17" s="28">
+        <f t="shared" si="26"/>
         <v>0.35</v>
       </c>
-      <c r="AK17" s="29">
-        <f>S$6/200+S13/200</f>
+      <c r="AK17" s="28">
+        <f t="shared" si="26"/>
         <v>0.47499999999999998</v>
       </c>
-      <c r="AL17" s="29">
-        <f>T$6/200+T13/200</f>
+      <c r="AL17" s="28">
+        <f t="shared" si="26"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="AM17" s="29">
-        <f>U$6/200+U13/200</f>
+      <c r="AM17" s="28">
+        <f t="shared" si="26"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AN17" s="29">
-        <f>V$6/200+V13/200</f>
+      <c r="AN17" s="28">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AO17" s="27" t="s">
+      <c r="AO17" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AP17" s="27" t="s">
+      <c r="AP17" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AQ17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>9.93</v>
       </c>
       <c r="BI17" t="s">
@@ -9394,43 +9395,43 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>12</v>
       </c>
-      <c r="O18" s="25"/>
-      <c r="AH18" s="29">
-        <f>P$6/200+P14/200</f>
+      <c r="O18" s="24"/>
+      <c r="AH18" s="28">
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AI18" s="29">
-        <f>Q$6/200+Q14/200</f>
+      <c r="AI18" s="28">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AJ18" s="29">
-        <f>R$6/200+R14/200</f>
+      <c r="AJ18" s="28">
+        <f t="shared" si="26"/>
         <v>0.1</v>
       </c>
-      <c r="AK18" s="29">
-        <f>S$6/200+S14/200</f>
+      <c r="AK18" s="28">
+        <f t="shared" si="26"/>
         <v>0.55000000000000004</v>
       </c>
-      <c r="AL18" s="29">
-        <f>T$6/200+T14/200</f>
+      <c r="AL18" s="28">
+        <f t="shared" si="26"/>
         <v>0.24</v>
       </c>
-      <c r="AM18" s="29">
-        <f>U$6/200+U14/200</f>
+      <c r="AM18" s="28">
+        <f t="shared" si="26"/>
         <v>0.105</v>
       </c>
-      <c r="AN18" s="29">
-        <f>V$6/200+V14/200</f>
+      <c r="AN18" s="28">
+        <f t="shared" si="26"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AO18" s="27" t="s">
+      <c r="AO18" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AP18" s="27" t="s">
+      <c r="AP18" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AQ18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>11.78</v>
       </c>
       <c r="BI18" t="s">
@@ -9461,43 +9462,43 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>15</v>
       </c>
-      <c r="O19" s="25"/>
-      <c r="AH19" s="29">
-        <f>P$7/200+P11/200</f>
-        <v>0.16999999999999998</v>
-      </c>
-      <c r="AI19" s="29">
-        <f>Q$7/200+Q11/200</f>
+      <c r="O19" s="24"/>
+      <c r="AH19" s="28">
+        <f>(P$7+P11)/200</f>
+        <v>0.17</v>
+      </c>
+      <c r="AI19" s="28">
+        <f t="shared" ref="AI19:AN22" si="28">(Q$7+Q11)/200</f>
         <v>0.5</v>
       </c>
-      <c r="AJ19" s="29">
-        <f>R$7/200+R11/200</f>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="AK19" s="29">
-        <f>S$7/200+S11/200</f>
+      <c r="AJ19" s="28">
+        <f t="shared" si="28"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AK19" s="28">
+        <f t="shared" si="28"/>
         <v>5.5E-2</v>
       </c>
-      <c r="AL19" s="29">
-        <f>T$7/200+T11/200</f>
+      <c r="AL19" s="28">
+        <f t="shared" si="28"/>
         <v>0.04</v>
       </c>
-      <c r="AM19" s="29">
-        <f>U$7/200+U11/200</f>
+      <c r="AM19" s="28">
+        <f t="shared" si="28"/>
         <v>0.01</v>
       </c>
-      <c r="AN19" s="29">
-        <f>V$7/200+V11/200</f>
+      <c r="AN19" s="28">
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AO19" s="28" t="s">
+      <c r="AO19" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="AP19" s="27" t="s">
+      <c r="AP19" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AQ19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>6.71</v>
       </c>
       <c r="BI19" t="s">
@@ -9528,44 +9529,44 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>18</v>
       </c>
-      <c r="O20" s="25"/>
-      <c r="AH20" s="29">
-        <f>P$7/200+P12/200</f>
+      <c r="O20" s="24"/>
+      <c r="AH20" s="28">
+        <f t="shared" ref="AH20:AH22" si="29">(P$7+P12)/200</f>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AI20" s="29">
-        <f>Q$7/200+Q12/200</f>
-        <v>0.32499999999999996</v>
-      </c>
-      <c r="AJ20" s="29">
-        <f>R$7/200+R12/200</f>
+      <c r="AI20" s="28">
+        <f t="shared" si="28"/>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="AJ20" s="28">
+        <f t="shared" si="28"/>
         <v>0.44500000000000001</v>
       </c>
-      <c r="AK20" s="29">
-        <f>S$7/200+S12/200</f>
+      <c r="AK20" s="28">
+        <f t="shared" si="28"/>
         <v>0.1</v>
       </c>
-      <c r="AL20" s="29">
-        <f>T$7/200+T12/200</f>
+      <c r="AL20" s="28">
+        <f t="shared" si="28"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="AM20" s="29">
-        <f>U$7/200+U12/200</f>
+      <c r="AM20" s="28">
+        <f t="shared" si="28"/>
         <v>0.01</v>
       </c>
-      <c r="AN20" s="29">
-        <f>V$7/200+V12/200</f>
+      <c r="AN20" s="28">
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AO20" s="28" t="s">
+      <c r="AO20" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="AP20" s="27" t="s">
+      <c r="AP20" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ20">
-        <f t="shared" si="5"/>
-        <v>7.55</v>
+        <f t="shared" si="13"/>
+        <v>7.5500000000000007</v>
       </c>
       <c r="BI20" t="s">
         <v>116</v>
@@ -9595,42 +9596,42 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>21</v>
       </c>
-      <c r="AH21" s="29">
-        <f>P$7/200+P13/200</f>
+      <c r="AH21" s="28">
+        <f t="shared" si="29"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AI21" s="29">
-        <f>Q$7/200+Q13/200</f>
+      <c r="AI21" s="28">
+        <f t="shared" si="28"/>
         <v>0.15</v>
       </c>
-      <c r="AJ21" s="29">
-        <f>R$7/200+R13/200</f>
+      <c r="AJ21" s="28">
+        <f t="shared" si="28"/>
         <v>0.42499999999999999</v>
       </c>
-      <c r="AK21" s="29">
-        <f>S$7/200+S13/200</f>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="AL21" s="29">
-        <f>T$7/200+T13/200</f>
+      <c r="AK21" s="28">
+        <f t="shared" si="28"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AL21" s="28">
+        <f t="shared" si="28"/>
         <v>0.09</v>
       </c>
-      <c r="AM21" s="29">
-        <f>U$7/200+U13/200</f>
+      <c r="AM21" s="28">
+        <f t="shared" si="28"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AN21" s="29">
-        <f>V$7/200+V13/200</f>
+      <c r="AN21" s="28">
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AO21" s="28" t="s">
+      <c r="AO21" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="AP21" s="27" t="s">
+      <c r="AP21" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AQ21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.6300000000000008</v>
       </c>
       <c r="BI21" t="s">
@@ -9661,42 +9662,42 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>24</v>
       </c>
-      <c r="AH22" s="29">
-        <f>P$7/200+P14/200</f>
+      <c r="AH22" s="28">
+        <f t="shared" si="29"/>
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="AI22" s="29">
-        <f>Q$7/200+Q14/200</f>
+      <c r="AI22" s="28">
+        <f t="shared" si="28"/>
         <v>0.15</v>
       </c>
-      <c r="AJ22" s="29">
-        <f>R$7/200+R14/200</f>
+      <c r="AJ22" s="28">
+        <f t="shared" si="28"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AK22" s="29">
-        <f>S$7/200+S14/200</f>
+      <c r="AK22" s="28">
+        <f t="shared" si="28"/>
         <v>0.3</v>
       </c>
-      <c r="AL22" s="29">
-        <f>T$7/200+T14/200</f>
+      <c r="AL22" s="28">
+        <f t="shared" si="28"/>
         <v>0.19</v>
       </c>
-      <c r="AM22" s="29">
-        <f>U$7/200+U14/200</f>
+      <c r="AM22" s="28">
+        <f t="shared" si="28"/>
         <v>0.105</v>
       </c>
-      <c r="AN22" s="29">
-        <f>V$7/200+V14/200</f>
+      <c r="AN22" s="28">
+        <f t="shared" si="28"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AO22" s="28" t="s">
+      <c r="AO22" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="AP22" s="27" t="s">
+      <c r="AP22" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AQ22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>10.480000000000002</v>
       </c>
       <c r="BI22" t="s">
@@ -9727,42 +9728,42 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>27</v>
       </c>
-      <c r="AH23" s="29">
-        <f>P$8/200+P11/200</f>
+      <c r="AH23" s="28">
+        <f>(P$8+P11)/200</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="AI23" s="29">
-        <f>Q$8/200+Q11/200</f>
-        <v>0.52499999999999991</v>
-      </c>
-      <c r="AJ23" s="29">
-        <f>R$8/200+R11/200</f>
+      <c r="AI23" s="28">
+        <f t="shared" ref="AI23:AN26" si="30">(Q$8+Q11)/200</f>
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="AJ23" s="28">
+        <f t="shared" si="30"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AK23" s="29">
-        <f>S$8/200+S11/200</f>
+      <c r="AK23" s="28">
+        <f t="shared" si="30"/>
         <v>5.5E-2</v>
       </c>
-      <c r="AL23" s="29">
-        <f>T$8/200+T11/200</f>
+      <c r="AL23" s="28">
+        <f t="shared" si="30"/>
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="AM23" s="29">
-        <f>U$8/200+U11/200</f>
+      <c r="AM23" s="28">
+        <f t="shared" si="30"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN23" s="29">
-        <f>V$8/200+V11/200</f>
+      <c r="AN23" s="28">
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AO23" s="28" t="s">
+      <c r="AO23" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="AP23" s="27" t="s">
+      <c r="AP23" s="26" t="s">
         <v>90</v>
       </c>
       <c r="AQ23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>6.6</v>
       </c>
       <c r="BI23" t="s">
@@ -9793,42 +9794,42 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>30</v>
       </c>
-      <c r="AH24" s="29">
-        <f>P$8/200+P12/200</f>
+      <c r="AH24" s="28">
+        <f t="shared" ref="AH24:AH26" si="31">(P$8+P12)/200</f>
         <v>0.1</v>
       </c>
-      <c r="AI24" s="29">
-        <f>Q$8/200+Q12/200</f>
+      <c r="AI24" s="28">
+        <f t="shared" si="30"/>
         <v>0.35</v>
       </c>
-      <c r="AJ24" s="29">
-        <f>R$8/200+R12/200</f>
+      <c r="AJ24" s="28">
+        <f t="shared" si="30"/>
         <v>0.39500000000000002</v>
       </c>
-      <c r="AK24" s="29">
-        <f>S$8/200+S12/200</f>
+      <c r="AK24" s="28">
+        <f t="shared" si="30"/>
         <v>0.1</v>
       </c>
-      <c r="AL24" s="29">
-        <f>T$8/200+T12/200</f>
+      <c r="AL24" s="28">
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
-      <c r="AM24" s="29">
-        <f>U$8/200+U12/200</f>
+      <c r="AM24" s="28">
+        <f t="shared" si="30"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AN24" s="29">
-        <f>V$8/200+V12/200</f>
+      <c r="AN24" s="28">
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AO24" s="28" t="s">
+      <c r="AO24" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="AP24" s="27" t="s">
+      <c r="AP24" s="26" t="s">
         <v>91</v>
       </c>
       <c r="AQ24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>7.44</v>
       </c>
       <c r="BI24" t="s">
@@ -9859,42 +9860,42 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>33</v>
       </c>
-      <c r="AH25" s="29">
-        <f>P$8/200+P13/200</f>
+      <c r="AH25" s="28">
+        <f t="shared" si="31"/>
         <v>0.1</v>
       </c>
-      <c r="AI25" s="29">
-        <f>Q$8/200+Q13/200</f>
+      <c r="AI25" s="28">
+        <f t="shared" si="30"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AJ25" s="29">
-        <f>R$8/200+R13/200</f>
+      <c r="AJ25" s="28">
+        <f t="shared" si="30"/>
         <v>0.375</v>
       </c>
-      <c r="AK25" s="29">
-        <f>S$8/200+S13/200</f>
-        <v>0.22499999999999998</v>
-      </c>
-      <c r="AL25" s="29">
-        <f>T$8/200+T13/200</f>
+      <c r="AK25" s="28">
+        <f t="shared" si="30"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="AL25" s="28">
+        <f t="shared" si="30"/>
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="AM25" s="29">
-        <f>U$8/200+U13/200</f>
+      <c r="AM25" s="28">
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
-      <c r="AN25" s="29">
-        <f>V$8/200+V13/200</f>
+      <c r="AN25" s="28">
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AO25" s="28" t="s">
+      <c r="AO25" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="AP25" s="27" t="s">
+      <c r="AP25" s="26" t="s">
         <v>92</v>
       </c>
       <c r="AQ25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>8.52</v>
       </c>
       <c r="BI25" t="s">
@@ -9925,42 +9926,42 @@
         <f>ROUNDUP(Tableau7[[#This Row],[Multiplicateur]]*VLOOKUP("Legendary",Tableau6[#All],2,FALSE),0)</f>
         <v>36</v>
       </c>
-      <c r="AH26" s="29">
-        <f>P$8/200+P14/200</f>
+      <c r="AH26" s="28">
+        <f t="shared" si="31"/>
         <v>0.1</v>
       </c>
-      <c r="AI26" s="29">
-        <f>Q$8/200+Q14/200</f>
+      <c r="AI26" s="28">
+        <f t="shared" si="30"/>
         <v>0.17499999999999999</v>
       </c>
-      <c r="AJ26" s="29">
-        <f>R$8/200+R14/200</f>
+      <c r="AJ26" s="28">
+        <f t="shared" si="30"/>
         <v>0.125</v>
       </c>
-      <c r="AK26" s="29">
-        <f>S$8/200+S14/200</f>
+      <c r="AK26" s="28">
+        <f t="shared" si="30"/>
         <v>0.3</v>
       </c>
-      <c r="AL26" s="29">
-        <f>T$8/200+T14/200</f>
+      <c r="AL26" s="28">
+        <f t="shared" si="30"/>
         <v>0.185</v>
       </c>
-      <c r="AM26" s="29">
-        <f>U$8/200+U14/200</f>
+      <c r="AM26" s="28">
+        <f t="shared" si="30"/>
         <v>0.11</v>
       </c>
-      <c r="AN26" s="29">
-        <f>V$8/200+V14/200</f>
+      <c r="AN26" s="28">
+        <f t="shared" si="30"/>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AO26" s="28" t="s">
+      <c r="AO26" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="AP26" s="27" t="s">
+      <c r="AP26" s="26" t="s">
         <v>99</v>
       </c>
       <c r="AQ26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>10.37</v>
       </c>
       <c r="BI26" t="s">
@@ -10269,15 +10270,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D561B29C098A574288915AA7FDCE85A0" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="250102bec12d8b142e58c1d00b1ffd8a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ee89e3b8-fbf6-4f90-a67d-b465f66f191f" xmlns:ns4="ab1f00cb-b678-48f7-aded-930f239c9527" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="440e872eed80589242d868d6c2b803d1" ns3:_="" ns4:_="">
     <xsd:import namespace="ee89e3b8-fbf6-4f90-a67d-b465f66f191f"/>
@@ -10480,6 +10472,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F126640-AE96-4D80-A3D5-B99E5C40D2BE}">
   <ds:schemaRefs>
@@ -10498,14 +10499,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5DF0EC-50CC-41C3-B7FF-8028A891B995}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10522,4 +10515,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22C65796-EE89-47E5-8B82-54AF3C286703}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>